<commit_message>
Baru ditamabahin sheet Variansi dan Standard Deviasi
</commit_message>
<xml_diff>
--- a/Data Penyebaran Data Frekuensi Tugas Kelompok.xlsx
+++ b/Data Penyebaran Data Frekuensi Tugas Kelompok.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22130"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hamdi\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ardy\OTW S1\SEMESTER 3\231-STATITISKA\statistika.git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{420C11F5-DB03-4C2A-AE49-6908D977DA66}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Simpangan Rata-rata" sheetId="3" r:id="rId3"/>
+    <sheet name="Variansi" sheetId="4" r:id="rId4"/>
+    <sheet name="Simpangan Baku Standard Deviasi" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="47">
   <si>
     <t>No. Urut</t>
   </si>
@@ -164,9 +165,6 @@
     <t>93 - 98</t>
   </si>
   <si>
-    <t>f</t>
-  </si>
-  <si>
     <t>x</t>
   </si>
   <si>
@@ -174,12 +172,15 @@
   </si>
   <si>
     <t>SR</t>
+  </si>
+  <si>
+    <t>Simpangan Rata-rata</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
@@ -334,7 +335,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="41" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -366,24 +367,30 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Comma [0] 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Comma [0] 2" xfId="5"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Normal 3" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
-    <cellStyle name="Normal 4" xfId="2" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
-    <cellStyle name="Normal 5" xfId="3" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 3" xfId="4"/>
+    <cellStyle name="Normal 4" xfId="2"/>
+    <cellStyle name="Normal 5" xfId="3"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -408,8 +415,8 @@
       <xdr:rowOff>185737</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1123952" cy="228589"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1">
@@ -507,7 +514,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1">
@@ -654,8 +661,8 @@
       <xdr:rowOff>157162</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="504826" cy="219163"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="TextBox 3">
@@ -697,6 +704,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -731,7 +739,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="TextBox 3">
@@ -796,8 +804,8 @@
       <xdr:rowOff>185737</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1123952" cy="228589"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="6" name="TextBox 5">
@@ -913,7 +921,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="6" name="TextBox 5">
@@ -1269,7 +1277,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1285,7 +1293,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
@@ -1293,7 +1301,7 @@
       </c>
     </row>
     <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="16"/>
+      <c r="A2" s="18"/>
       <c r="B2" s="8" t="s">
         <v>2</v>
       </c>
@@ -1938,11 +1946,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40EAE36B-7214-4C08-949E-AEAD6D68855E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:R15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M7" sqref="M7:N15"/>
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2152,18 +2160,18 @@
       </c>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="M7" s="17" t="s">
+      <c r="M7" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="N7" s="17" t="s">
+      <c r="N7" s="15" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="M8" s="17" t="s">
+      <c r="M8" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="N8" s="17">
+      <c r="N8" s="15">
         <v>3</v>
       </c>
     </row>
@@ -2171,10 +2179,10 @@
       <c r="B9" t="s">
         <v>27</v>
       </c>
-      <c r="M9" s="17" t="s">
+      <c r="M9" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="N9" s="17">
+      <c r="N9" s="15">
         <v>2</v>
       </c>
     </row>
@@ -2209,10 +2217,10 @@
       <c r="K10" s="6">
         <v>79.666666666666671</v>
       </c>
-      <c r="M10" s="17" t="s">
+      <c r="M10" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="N10" s="17">
+      <c r="N10" s="15">
         <v>2</v>
       </c>
     </row>
@@ -2247,7 +2255,7 @@
       <c r="K11" s="5">
         <v>86.133333333333326</v>
       </c>
-      <c r="M11" s="17" t="s">
+      <c r="M11" s="15" t="s">
         <v>39</v>
       </c>
       <c r="N11" s="5">
@@ -2285,10 +2293,10 @@
       <c r="K12" s="5">
         <v>90.666666666666671</v>
       </c>
-      <c r="M12" s="17" t="s">
+      <c r="M12" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="N12" s="17">
+      <c r="N12" s="15">
         <v>11</v>
       </c>
     </row>
@@ -2323,10 +2331,10 @@
       <c r="K13" s="5">
         <v>93.2</v>
       </c>
-      <c r="M13" s="17" t="s">
+      <c r="M13" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="N13" s="17">
+      <c r="N13" s="15">
         <v>15</v>
       </c>
     </row>
@@ -2361,18 +2369,18 @@
       <c r="K14" s="5">
         <v>97.066666666666663</v>
       </c>
-      <c r="M14" s="17" t="s">
+      <c r="M14" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="N14" s="17">
+      <c r="N14" s="15">
         <v>13</v>
       </c>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="M15" s="17" t="s">
+      <c r="M15" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="N15" s="17">
+      <c r="N15" s="15">
         <f>SUM(N8:N14)</f>
         <v>50</v>
       </c>
@@ -2383,11 +2391,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31A3B53D-6A7D-4E7E-9A0E-0737B85E87A9}">
-  <dimension ref="B1:G17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2397,216 +2405,208 @@
     <col min="7" max="7" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D1" t="s">
-        <v>44</v>
-      </c>
-    </row>
     <row r="2" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="D5" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="E5" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="17">
+      <c r="C6" s="15">
         <v>3</v>
       </c>
-      <c r="D6" s="18">
+      <c r="D6" s="16">
         <f>(62+57)/2</f>
         <v>59.5</v>
       </c>
-      <c r="E6" s="18">
+      <c r="E6" s="16">
         <f>C6*D6</f>
         <v>178.5</v>
       </c>
-      <c r="F6" s="18">
+      <c r="F6" s="16">
         <f>(ABS(D6-$D$16))</f>
         <v>25.799999999999997</v>
       </c>
-      <c r="G6" s="18">
+      <c r="G6" s="16">
         <f>C6*F6</f>
         <v>77.399999999999991</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="17">
+      <c r="C7" s="15">
         <v>2</v>
       </c>
-      <c r="D7" s="18">
+      <c r="D7" s="16">
         <f>(68 + 63)/2</f>
         <v>65.5</v>
       </c>
-      <c r="E7" s="18">
+      <c r="E7" s="16">
         <f t="shared" ref="E7:E12" si="0">C7*D7</f>
         <v>131</v>
       </c>
-      <c r="F7" s="18">
+      <c r="F7" s="16">
         <f t="shared" ref="F7:F12" si="1">(ABS(D7-$D$16))</f>
         <v>19.799999999999997</v>
       </c>
-      <c r="G7" s="18">
+      <c r="G7" s="16">
         <f t="shared" ref="G7:G12" si="2">C7*F7</f>
         <v>39.599999999999994</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="17">
+      <c r="C8" s="15">
         <v>2</v>
       </c>
-      <c r="D8" s="18">
+      <c r="D8" s="16">
         <f>(74 + 69)/2</f>
         <v>71.5</v>
       </c>
-      <c r="E8" s="18">
+      <c r="E8" s="16">
         <f t="shared" si="0"/>
         <v>143</v>
       </c>
-      <c r="F8" s="18">
+      <c r="F8" s="16">
         <f t="shared" si="1"/>
         <v>13.799999999999997</v>
       </c>
-      <c r="G8" s="18">
+      <c r="G8" s="16">
         <f t="shared" si="2"/>
         <v>27.599999999999994</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="15" t="s">
         <v>39</v>
       </c>
       <c r="C9" s="5">
         <v>4</v>
       </c>
-      <c r="D9" s="18">
+      <c r="D9" s="16">
         <f>(80 + 75)/ 2</f>
         <v>77.5</v>
       </c>
-      <c r="E9" s="18">
+      <c r="E9" s="16">
         <f t="shared" si="0"/>
         <v>310</v>
       </c>
-      <c r="F9" s="18">
+      <c r="F9" s="16">
         <f t="shared" si="1"/>
         <v>7.7999999999999972</v>
       </c>
-      <c r="G9" s="18">
+      <c r="G9" s="16">
         <f t="shared" si="2"/>
         <v>31.199999999999989</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="C10" s="17">
+      <c r="C10" s="15">
         <v>11</v>
       </c>
-      <c r="D10" s="18">
+      <c r="D10" s="16">
         <f>(81+86)/2</f>
         <v>83.5</v>
       </c>
-      <c r="E10" s="18">
+      <c r="E10" s="16">
         <f t="shared" si="0"/>
         <v>918.5</v>
       </c>
-      <c r="F10" s="18">
+      <c r="F10" s="16">
         <f t="shared" si="1"/>
         <v>1.7999999999999972</v>
       </c>
-      <c r="G10" s="18">
+      <c r="G10" s="16">
         <f t="shared" si="2"/>
         <v>19.799999999999969</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="C11" s="17">
+      <c r="C11" s="15">
         <v>15</v>
       </c>
-      <c r="D11" s="18">
+      <c r="D11" s="16">
         <f>(87+92)/2</f>
         <v>89.5</v>
       </c>
-      <c r="E11" s="18">
+      <c r="E11" s="16">
         <f t="shared" si="0"/>
         <v>1342.5</v>
       </c>
-      <c r="F11" s="18">
+      <c r="F11" s="16">
         <f t="shared" si="1"/>
         <v>4.2000000000000028</v>
       </c>
-      <c r="G11" s="18">
+      <c r="G11" s="16">
         <f t="shared" si="2"/>
         <v>63.000000000000043</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="17" t="s">
+      <c r="B12" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="C12" s="17">
+      <c r="C12" s="15">
         <v>13</v>
       </c>
-      <c r="D12" s="18">
+      <c r="D12" s="16">
         <f>(93+98)/2</f>
         <v>95.5</v>
       </c>
-      <c r="E12" s="18">
+      <c r="E12" s="16">
         <f t="shared" si="0"/>
         <v>1241.5</v>
       </c>
-      <c r="F12" s="18">
+      <c r="F12" s="16">
         <f t="shared" si="1"/>
         <v>10.200000000000003</v>
       </c>
-      <c r="G12" s="18">
+      <c r="G12" s="16">
         <f t="shared" si="2"/>
         <v>132.60000000000002</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="17">
+      <c r="C13" s="15">
         <f>SUM(C6:C12)</f>
         <v>50</v>
       </c>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18">
+      <c r="D13" s="16"/>
+      <c r="E13" s="16">
         <f>SUM(E6:E12)</f>
         <v>4265</v>
       </c>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18">
+      <c r="F13" s="16"/>
+      <c r="G13" s="16">
         <f>SUM(G6:G12)</f>
         <v>391.2</v>
       </c>
@@ -2617,9 +2617,13 @@
         <v>85.3</v>
       </c>
     </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C17" t="s">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="20" t="s">
         <v>46</v>
+      </c>
+      <c r="B17" s="20"/>
+      <c r="C17" s="19" t="s">
+        <v>45</v>
       </c>
       <c r="D17">
         <f>G13/C13</f>
@@ -2627,8 +2631,37 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A17:B17"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Excel dan Powerpoint update again
</commit_message>
<xml_diff>
--- a/Data Penyebaran Data Frekuensi Tugas Kelompok.xlsx
+++ b/Data Penyebaran Data Frekuensi Tugas Kelompok.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22130"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ardy\OTW S1\SEMESTER 3\231-STATITISKA\statistika.git\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Wildan\SEMESTER 3\STATISTIKA (231)\PowerPoint\statistika.git\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB424A39-5F07-47FC-B96B-C6FEAE9D2F15}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +19,7 @@
     <sheet name="Variansi" sheetId="4" r:id="rId4"/>
     <sheet name="Simpangan Baku Standard Deviasi" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -180,9 +181,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -333,7 +334,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="41" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -371,6 +372,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -378,19 +382,16 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Comma [0] 2" xfId="5"/>
+    <cellStyle name="Comma [0] 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
-    <cellStyle name="Normal 3" xfId="4"/>
-    <cellStyle name="Normal 4" xfId="2"/>
-    <cellStyle name="Normal 5" xfId="3"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 3" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Normal 4" xfId="2" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Normal 5" xfId="3" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1277,11 +1278,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:B13"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1293,7 +1294,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
@@ -1301,7 +1302,7 @@
       </c>
     </row>
     <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="18"/>
+      <c r="A2" s="19"/>
       <c r="B2" s="8" t="s">
         <v>2</v>
       </c>
@@ -1946,11 +1947,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:R15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2391,7 +2392,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A2:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2622,7 +2623,7 @@
         <v>46</v>
       </c>
       <c r="B17" s="20"/>
-      <c r="C17" s="19" t="s">
+      <c r="C17" s="17" t="s">
         <v>45</v>
       </c>
       <c r="D17">
@@ -2641,7 +2642,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2655,10 +2656,10 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>

<commit_message>
Standar Deviasi / SImpangan baku Clear
</commit_message>
<xml_diff>
--- a/Data Penyebaran Data Frekuensi Tugas Kelompok.xlsx
+++ b/Data Penyebaran Data Frekuensi Tugas Kelompok.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22130"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Wildan\SEMESTER 3\STATISTIKA (231)\PowerPoint\statistika.git\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ardy\OTW S1\SEMESTER 3\231-STATITISKA\statistika\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB424A39-5F07-47FC-B96B-C6FEAE9D2F15}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +18,7 @@
     <sheet name="Variansi" sheetId="4" r:id="rId4"/>
     <sheet name="Simpangan Baku Standard Deviasi" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="49">
   <si>
     <t>No. Urut</t>
   </si>
@@ -176,16 +175,45 @@
   </si>
   <si>
     <t>Simpangan Rata-rata</t>
+  </si>
+  <si>
+    <r>
+      <t>S</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">2 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> =</t>
+    </r>
+  </si>
+  <si>
+    <t>S    =</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -245,6 +273,21 @@
       <name val="Calibri Light"/>
       <family val="1"/>
       <scheme val="major"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -334,9 +377,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -384,14 +427,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Comma [0] 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Comma [0] 2" xfId="5"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Normal 3" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
-    <cellStyle name="Normal 4" xfId="2" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
-    <cellStyle name="Normal 5" xfId="3" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 3" xfId="4"/>
+    <cellStyle name="Normal 4" xfId="2"/>
+    <cellStyle name="Normal 5" xfId="3"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1011,6 +1055,589 @@
         </xdr:sp>
       </mc:Fallback>
     </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>38098</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>185737</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1123952" cy="228589"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2" name="TextBox 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA8E659C-447D-4EE3-9972-EFFCA70A3FCD}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3086098" y="566737"/>
+              <a:ext cx="1123952" cy="228589"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1400" b="0">
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>|</a:t>
+              </a:r>
+              <a14:m>
+                <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:r>
+                    <a:rPr lang="en-US" sz="1400" b="0" i="1">
+                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                    </a:rPr>
+                    <m:t>𝑥</m:t>
+                  </m:r>
+                  <m:r>
+                    <a:rPr lang="en-US" sz="1400" b="0" i="1">
+                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                    </a:rPr>
+                    <m:t>−</m:t>
+                  </m:r>
+                  <m:acc>
+                    <m:accPr>
+                      <m:chr m:val="̅"/>
+                      <m:ctrlPr>
+                        <a:rPr lang="en-ID" sz="1400" i="1">
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        </a:rPr>
+                      </m:ctrlPr>
+                    </m:accPr>
+                    <m:e>
+                      <m:r>
+                        <a:rPr lang="en-ID" sz="1400" i="1">
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        </a:rPr>
+                        <m:t>𝑥</m:t>
+                      </m:r>
+                      <m:r>
+                        <a:rPr lang="en-US" sz="1400" b="0" i="1">
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        </a:rPr>
+                        <m:t>|</m:t>
+                      </m:r>
+                    </m:e>
+                  </m:acc>
+                </m:oMath>
+              </a14:m>
+              <a:endParaRPr lang="en-ID" sz="1600"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2" name="TextBox 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA8E659C-447D-4EE3-9972-EFFCA70A3FCD}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3086098" y="566737"/>
+              <a:ext cx="1123952" cy="228589"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1400" b="0">
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>|</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1400" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑥−</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-ID" sz="1400" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>(𝑥</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1400" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>|</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-ID" sz="1400" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>) ̅</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-ID" sz="1600"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="981075" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{889B8C32-F756-4670-958A-4B4379E11561}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5276850" y="647700"/>
+          <a:ext cx="981075" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-ID" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="398507" cy="316497"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="4" name="TextBox 3"/>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="4657725" y="1514475"/>
+              <a:ext cx="398507" cy="316497"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:rad>
+                      <m:radPr>
+                        <m:degHide m:val="on"/>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1600" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:radPr>
+                      <m:deg/>
+                      <m:e>
+                        <m:sSup>
+                          <m:sSupPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-US" sz="1600" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSupPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1600" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑠</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sup>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1600" i="0">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>2</m:t>
+                            </m:r>
+                          </m:sup>
+                        </m:sSup>
+                      </m:e>
+                    </m:rad>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="4" name="TextBox 3"/>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="4657725" y="1514475"/>
+              <a:ext cx="398507" cy="316497"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="en-US" sz="1600" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>√(𝑠^2 )</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1036181" cy="298159"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="5" name="TextBox 4"/>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="4657725" y="1981200"/>
+              <a:ext cx="1036181" cy="298159"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:rad>
+                      <m:radPr>
+                        <m:degHide m:val="on"/>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1600" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:radPr>
+                      <m:deg/>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1600">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>300312,5</m:t>
+                        </m:r>
+                      </m:e>
+                    </m:rad>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="5" name="TextBox 4"/>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="4657725" y="1981200"/>
+              <a:ext cx="1036181" cy="298159"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="en-US" sz="1600" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>√300312,5</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="987835" cy="250453"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="TextBox 5"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4772025" y="2409825"/>
+          <a:ext cx="987835" cy="250453"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600"/>
+            <a:t>548.007755</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
 </xdr:wsDr>
@@ -1278,7 +1905,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1947,10 +2574,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:R15"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
@@ -2392,7 +3019,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2642,7 +3269,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2656,13 +3283,213 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B4:I13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1:O1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="8" width="9.140625" style="2"/>
+    <col min="9" max="9" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B4" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="F4" s="16"/>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B5" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="15">
+        <v>3</v>
+      </c>
+      <c r="D5" s="16">
+        <f>(62+57)/2</f>
+        <v>59.5</v>
+      </c>
+      <c r="E5" s="16">
+        <f>C5*D5</f>
+        <v>178.5</v>
+      </c>
+      <c r="F5" s="16">
+        <f>(ABS(D5-$D$16))</f>
+        <v>59.5</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B6" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="15">
+        <v>2</v>
+      </c>
+      <c r="D6" s="16">
+        <f>(68 + 63)/2</f>
+        <v>65.5</v>
+      </c>
+      <c r="E6" s="16">
+        <f t="shared" ref="E6:E11" si="0">C6*D6</f>
+        <v>131</v>
+      </c>
+      <c r="F6" s="16">
+        <f t="shared" ref="F6:F11" si="1">(ABS(D6-$D$16))</f>
+        <v>65.5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B7" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="15">
+        <v>2</v>
+      </c>
+      <c r="D7" s="16">
+        <f>(74 + 69)/2</f>
+        <v>71.5</v>
+      </c>
+      <c r="E7" s="16">
+        <f t="shared" si="0"/>
+        <v>143</v>
+      </c>
+      <c r="F7" s="16">
+        <f t="shared" si="1"/>
+        <v>71.5</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="I7" s="2">
+        <f>C12*(F12^2)/(C12-1)</f>
+        <v>300312.5</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B8" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="5">
+        <v>4</v>
+      </c>
+      <c r="D8" s="16">
+        <f>(80 + 75)/ 2</f>
+        <v>77.5</v>
+      </c>
+      <c r="E8" s="16">
+        <f t="shared" si="0"/>
+        <v>310</v>
+      </c>
+      <c r="F8" s="16">
+        <f t="shared" si="1"/>
+        <v>77.5</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B9" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="15">
+        <v>11</v>
+      </c>
+      <c r="D9" s="16">
+        <f>(81+86)/2</f>
+        <v>83.5</v>
+      </c>
+      <c r="E9" s="16">
+        <f t="shared" si="0"/>
+        <v>918.5</v>
+      </c>
+      <c r="F9" s="16">
+        <f t="shared" si="1"/>
+        <v>83.5</v>
+      </c>
+      <c r="H9" s="21" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B10" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="15">
+        <v>15</v>
+      </c>
+      <c r="D10" s="16">
+        <f>(87+92)/2</f>
+        <v>89.5</v>
+      </c>
+      <c r="E10" s="16">
+        <f t="shared" si="0"/>
+        <v>1342.5</v>
+      </c>
+      <c r="F10" s="16">
+        <f t="shared" si="1"/>
+        <v>89.5</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B11" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="15">
+        <v>13</v>
+      </c>
+      <c r="D11" s="16">
+        <f>(93+98)/2</f>
+        <v>95.5</v>
+      </c>
+      <c r="E11" s="16">
+        <f t="shared" si="0"/>
+        <v>1241.5</v>
+      </c>
+      <c r="F11" s="16">
+        <f t="shared" si="1"/>
+        <v>95.5</v>
+      </c>
+      <c r="H11" s="21" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B12" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="15">
+        <f>SUM(C5:C11)</f>
+        <v>50</v>
+      </c>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16">
+        <f>SUM(E5:E11)</f>
+        <v>4265</v>
+      </c>
+      <c r="F12" s="16">
+        <f>SUM(F5:F11)</f>
+        <v>542.5</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="H13" s="21" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update standar deviasi nih gan
</commit_message>
<xml_diff>
--- a/Data Penyebaran Data Frekuensi Tugas Kelompok.xlsx
+++ b/Data Penyebaran Data Frekuensi Tugas Kelompok.xlsx
@@ -9,14 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Data Frekuensi" sheetId="2" r:id="rId2"/>
     <sheet name="Simpangan Rata-rata" sheetId="3" r:id="rId3"/>
     <sheet name="Variansi" sheetId="4" r:id="rId4"/>
     <sheet name="Simpangan Baku Standard Deviasi" sheetId="5" r:id="rId5"/>
+    <sheet name="Jangkauan Kuartil" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="50">
   <si>
     <t>No. Urut</t>
   </si>
@@ -205,6 +206,32 @@
   <si>
     <t>S    =</t>
   </si>
+  <si>
+    <r>
+      <t>S</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">2 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> =</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -213,7 +240,7 @@
   <numFmts count="1">
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -284,6 +311,21 @@
     </font>
     <font>
       <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="16"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -379,7 +421,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="41" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -418,6 +460,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -427,7 +470,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Comma [0] 2" xfId="5"/>
@@ -1308,6 +1351,257 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>38098</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>185737</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1123952" cy="228589"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2" name="TextBox 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA8E659C-447D-4EE3-9972-EFFCA70A3FCD}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3086098" y="566737"/>
+              <a:ext cx="1123952" cy="228589"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1400" b="0">
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>|</a:t>
+              </a:r>
+              <a14:m>
+                <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:r>
+                    <a:rPr lang="en-US" sz="1400" b="0" i="1">
+                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                    </a:rPr>
+                    <m:t>𝑥</m:t>
+                  </m:r>
+                  <m:r>
+                    <a:rPr lang="en-US" sz="1400" b="0" i="1">
+                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                    </a:rPr>
+                    <m:t>−</m:t>
+                  </m:r>
+                  <m:acc>
+                    <m:accPr>
+                      <m:chr m:val="̅"/>
+                      <m:ctrlPr>
+                        <a:rPr lang="en-ID" sz="1400" i="1">
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        </a:rPr>
+                      </m:ctrlPr>
+                    </m:accPr>
+                    <m:e>
+                      <m:r>
+                        <a:rPr lang="en-ID" sz="1400" i="1">
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        </a:rPr>
+                        <m:t>𝑥</m:t>
+                      </m:r>
+                      <m:r>
+                        <a:rPr lang="en-US" sz="1400" b="0" i="1">
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        </a:rPr>
+                        <m:t>|</m:t>
+                      </m:r>
+                    </m:e>
+                  </m:acc>
+                </m:oMath>
+              </a14:m>
+              <a:endParaRPr lang="en-ID" sz="1600"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2" name="TextBox 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA8E659C-447D-4EE3-9972-EFFCA70A3FCD}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3086098" y="566737"/>
+              <a:ext cx="1123952" cy="228589"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1400" b="0">
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>|</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1400" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑥−</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-ID" sz="1400" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>(𝑥</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1400" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>|</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-ID" sz="1400" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>) ̅</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-ID" sz="1600"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="981075" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{889B8C32-F756-4670-958A-4B4379E11561}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5276850" y="647700"/>
+          <a:ext cx="981075" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-ID" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
@@ -1316,8 +1610,8 @@
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="398507" cy="316497"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="TextBox 3"/>
@@ -1406,7 +1700,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="TextBox 3"/>
@@ -1465,8 +1759,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1036181" cy="298159"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="TextBox 4"/>
@@ -1536,7 +1830,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="TextBox 4"/>
@@ -1921,7 +2215,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
@@ -1929,7 +2223,7 @@
       </c>
     </row>
     <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="19"/>
+      <c r="A2" s="20"/>
       <c r="B2" s="8" t="s">
         <v>2</v>
       </c>
@@ -2578,7 +2872,7 @@
   <dimension ref="B1:R15"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="Q5" sqref="Q5"/>
+      <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3246,10 +3540,10 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="20" t="s">
+      <c r="A17" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="B17" s="20"/>
+      <c r="B17" s="21"/>
       <c r="C17" s="17" t="s">
         <v>45</v>
       </c>
@@ -3270,24 +3564,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B4:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:I13"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1:O1048576"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3352,7 +3632,7 @@
         <v>65.5</v>
       </c>
     </row>
-    <row r="7" spans="2:9" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B7" s="15" t="s">
         <v>38</v>
       </c>
@@ -3371,10 +3651,10 @@
         <f t="shared" si="1"/>
         <v>71.5</v>
       </c>
-      <c r="H7" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="I7" s="2">
+      <c r="H7" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="I7" s="18">
         <f>C12*(F12^2)/(C12-1)</f>
         <v>300312.5</v>
       </c>
@@ -3418,9 +3698,7 @@
         <f t="shared" si="1"/>
         <v>83.5</v>
       </c>
-      <c r="H9" s="21" t="s">
-        <v>48</v>
-      </c>
+      <c r="H9" s="18"/>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="15" t="s">
@@ -3461,9 +3739,7 @@
         <f t="shared" si="1"/>
         <v>95.5</v>
       </c>
-      <c r="H11" s="21" t="s">
-        <v>48</v>
-      </c>
+      <c r="H11" s="18"/>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" s="15" t="s">
@@ -3484,7 +3760,218 @@
       </c>
     </row>
     <row r="13" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="H13" s="21" t="s">
+      <c r="H13" s="18"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B4:I13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D16" sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="8" width="9.140625" style="2"/>
+    <col min="9" max="9" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B4" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="F4" s="16"/>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B5" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="15">
+        <v>3</v>
+      </c>
+      <c r="D5" s="16">
+        <f>(62+57)/2</f>
+        <v>59.5</v>
+      </c>
+      <c r="E5" s="16">
+        <f>C5*D5</f>
+        <v>178.5</v>
+      </c>
+      <c r="F5" s="16">
+        <f>(ABS(D5-$D$16))</f>
+        <v>59.5</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B6" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="15">
+        <v>2</v>
+      </c>
+      <c r="D6" s="16">
+        <f>(68 + 63)/2</f>
+        <v>65.5</v>
+      </c>
+      <c r="E6" s="16">
+        <f t="shared" ref="E6:E11" si="0">C6*D6</f>
+        <v>131</v>
+      </c>
+      <c r="F6" s="16">
+        <f t="shared" ref="F6:F11" si="1">(ABS(D6-$D$16))</f>
+        <v>65.5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B7" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="15">
+        <v>2</v>
+      </c>
+      <c r="D7" s="16">
+        <f>(74 + 69)/2</f>
+        <v>71.5</v>
+      </c>
+      <c r="E7" s="16">
+        <f t="shared" si="0"/>
+        <v>143</v>
+      </c>
+      <c r="F7" s="16">
+        <f t="shared" si="1"/>
+        <v>71.5</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="I7" s="2">
+        <f>C12*(F12^2)/(C12-1)</f>
+        <v>300312.5</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B8" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="5">
+        <v>4</v>
+      </c>
+      <c r="D8" s="16">
+        <f>(80 + 75)/ 2</f>
+        <v>77.5</v>
+      </c>
+      <c r="E8" s="16">
+        <f t="shared" si="0"/>
+        <v>310</v>
+      </c>
+      <c r="F8" s="16">
+        <f t="shared" si="1"/>
+        <v>77.5</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B9" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="15">
+        <v>11</v>
+      </c>
+      <c r="D9" s="16">
+        <f>(81+86)/2</f>
+        <v>83.5</v>
+      </c>
+      <c r="E9" s="16">
+        <f t="shared" si="0"/>
+        <v>918.5</v>
+      </c>
+      <c r="F9" s="16">
+        <f t="shared" si="1"/>
+        <v>83.5</v>
+      </c>
+      <c r="H9" s="18" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B10" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="15">
+        <v>15</v>
+      </c>
+      <c r="D10" s="16">
+        <f>(87+92)/2</f>
+        <v>89.5</v>
+      </c>
+      <c r="E10" s="16">
+        <f t="shared" si="0"/>
+        <v>1342.5</v>
+      </c>
+      <c r="F10" s="16">
+        <f t="shared" si="1"/>
+        <v>89.5</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B11" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="15">
+        <v>13</v>
+      </c>
+      <c r="D11" s="16">
+        <f>(93+98)/2</f>
+        <v>95.5</v>
+      </c>
+      <c r="E11" s="16">
+        <f t="shared" si="0"/>
+        <v>1241.5</v>
+      </c>
+      <c r="F11" s="16">
+        <f t="shared" si="1"/>
+        <v>95.5</v>
+      </c>
+      <c r="H11" s="18" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B12" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="15">
+        <f>SUM(C5:C11)</f>
+        <v>50</v>
+      </c>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16">
+        <f>SUM(E5:E11)</f>
+        <v>4265</v>
+      </c>
+      <c r="F12" s="16">
+        <f>SUM(F5:F11)</f>
+        <v>542.5</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="H13" s="18" t="s">
         <v>48</v>
       </c>
     </row>
@@ -3492,4 +3979,18 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
penambahan jangkauan kuartil dan persentil di excel penambahan simpangan rata-rata dan variansi di ppt
</commit_message>
<xml_diff>
--- a/Data Penyebaran Data Frekuensi Tugas Kelompok.xlsx
+++ b/Data Penyebaran Data Frekuensi Tugas Kelompok.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22130"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ardy\OTW S1\SEMESTER 3\231-STATITISKA\statistika\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hamdi\Documents\statistikafiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{569A81FC-58ED-4C46-996E-5FC0675AC8D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="45" windowWidth="20490" windowHeight="10875" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,8 +19,9 @@
     <sheet name="Variansi" sheetId="4" r:id="rId4"/>
     <sheet name="Simpangan Baku Standard Deviasi" sheetId="5" r:id="rId5"/>
     <sheet name="Jangkauan Kuartil" sheetId="6" r:id="rId6"/>
+    <sheet name="Jangkauan Persentil" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="64">
   <si>
     <t>No. Urut</t>
   </si>
@@ -232,13 +234,55 @@
       <t xml:space="preserve"> =</t>
     </r>
   </si>
+  <si>
+    <t>interval</t>
+  </si>
+  <si>
+    <t>Kelas Ke-5 (81-86)</t>
+  </si>
+  <si>
+    <t>Kelas Ke-7 (93-98)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jumlah Q1 </t>
+  </si>
+  <si>
+    <t>Jumlah Q3</t>
+  </si>
+  <si>
+    <t>Jangkauan Persentil</t>
+  </si>
+  <si>
+    <t>Kelas Q1 berada di periode</t>
+  </si>
+  <si>
+    <t>Kelas Q3 berada di periode</t>
+  </si>
+  <si>
+    <t>Kelas P10 Berada pada periode</t>
+  </si>
+  <si>
+    <t>Kelas P90 Berada pada periode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jumlah P10 </t>
+  </si>
+  <si>
+    <t>Kelas ke 2 (63-68)</t>
+  </si>
+  <si>
+    <t>Kelas ke 7 (93-98)</t>
+  </si>
+  <si>
+    <t>Jumlah P90</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="13" x14ac:knownFonts="1">
     <font>
@@ -352,7 +396,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -412,6 +456,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -419,9 +472,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="41" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -461,6 +514,38 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -470,15 +555,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Comma [0] 2" xfId="5"/>
+    <cellStyle name="Comma [0] 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
-    <cellStyle name="Normal 3" xfId="4"/>
-    <cellStyle name="Normal 4" xfId="2"/>
-    <cellStyle name="Normal 5" xfId="3"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 3" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Normal 4" xfId="2" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Normal 5" xfId="3" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -510,7 +594,7 @@
             <xdr:cNvPr id="2" name="TextBox 1">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{064A5368-0754-4CC2-984A-AB4897E3E26B}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -699,7 +783,7 @@
         <xdr:cNvPr id="3" name="TextBox 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{39BD638F-98F2-4CEB-9CCA-E5938AEF0D78}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -756,7 +840,7 @@
             <xdr:cNvPr id="4" name="TextBox 3">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E3E3D377-920B-42C7-986F-78EA2BE97E09}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -899,7 +983,7 @@
             <xdr:cNvPr id="6" name="TextBox 5">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{08F78429-826A-4051-8D02-6D1612D41A68}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000006000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1113,257 +1197,6 @@
       <xdr:rowOff>185737</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1123952" cy="228589"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="2" name="TextBox 1">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA8E659C-447D-4EE3-9972-EFFCA70A3FCD}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr txBox="1"/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="3086098" y="566737"/>
-              <a:ext cx="1123952" cy="228589"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:lnRef>
-            <a:fillRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:r>
-                <a:rPr lang="en-US" sz="1400" b="0">
-                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>|</a:t>
-              </a:r>
-              <a14:m>
-                <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
-                  <m:r>
-                    <a:rPr lang="en-US" sz="1400" b="0" i="1">
-                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                      <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                    </a:rPr>
-                    <m:t>𝑥</m:t>
-                  </m:r>
-                  <m:r>
-                    <a:rPr lang="en-US" sz="1400" b="0" i="1">
-                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                      <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                    </a:rPr>
-                    <m:t>−</m:t>
-                  </m:r>
-                  <m:acc>
-                    <m:accPr>
-                      <m:chr m:val="̅"/>
-                      <m:ctrlPr>
-                        <a:rPr lang="en-ID" sz="1400" i="1">
-                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                        </a:rPr>
-                      </m:ctrlPr>
-                    </m:accPr>
-                    <m:e>
-                      <m:r>
-                        <a:rPr lang="en-ID" sz="1400" i="1">
-                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                        </a:rPr>
-                        <m:t>𝑥</m:t>
-                      </m:r>
-                      <m:r>
-                        <a:rPr lang="en-US" sz="1400" b="0" i="1">
-                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                        </a:rPr>
-                        <m:t>|</m:t>
-                      </m:r>
-                    </m:e>
-                  </m:acc>
-                </m:oMath>
-              </a14:m>
-              <a:endParaRPr lang="en-ID" sz="1600"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Choice>
-      <mc:Fallback>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="2" name="TextBox 1">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA8E659C-447D-4EE3-9972-EFFCA70A3FCD}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr txBox="1"/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="3086098" y="566737"/>
-              <a:ext cx="1123952" cy="228589"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:lnRef>
-            <a:fillRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:r>
-                <a:rPr lang="en-US" sz="1400" b="0">
-                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>|</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-US" sz="1400" b="0" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>𝑥−</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-ID" sz="1400" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>(𝑥</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-US" sz="1400" b="0" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>|</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-ID" sz="1400" b="0" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>) ̅</a:t>
-              </a:r>
-              <a:endParaRPr lang="en-ID" sz="1600"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>400050</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="981075" cy="264560"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="TextBox 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{889B8C32-F756-4670-958A-4B4379E11561}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5276850" y="647700"/>
-          <a:ext cx="981075" cy="264560"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
-          <a:spAutoFit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:endParaRPr lang="en-ID" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>38098</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>185737</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="1123952" cy="228589"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
       <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
@@ -1371,7 +1204,7 @@
             <xdr:cNvPr id="2" name="TextBox 1">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA8E659C-447D-4EE3-9972-EFFCA70A3FCD}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1560,7 +1393,258 @@
         <xdr:cNvPr id="3" name="TextBox 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{889B8C32-F756-4670-958A-4B4379E11561}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5276850" y="647700"/>
+          <a:ext cx="981075" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-ID" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>38098</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>185737</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1123952" cy="228589"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2" name="TextBox 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3086098" y="566737"/>
+              <a:ext cx="1123952" cy="228589"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1400" b="0">
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>|</a:t>
+              </a:r>
+              <a14:m>
+                <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:r>
+                    <a:rPr lang="en-US" sz="1400" b="0" i="1">
+                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                    </a:rPr>
+                    <m:t>𝑥</m:t>
+                  </m:r>
+                  <m:r>
+                    <a:rPr lang="en-US" sz="1400" b="0" i="1">
+                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                    </a:rPr>
+                    <m:t>−</m:t>
+                  </m:r>
+                  <m:acc>
+                    <m:accPr>
+                      <m:chr m:val="̅"/>
+                      <m:ctrlPr>
+                        <a:rPr lang="en-ID" sz="1400" i="1">
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        </a:rPr>
+                      </m:ctrlPr>
+                    </m:accPr>
+                    <m:e>
+                      <m:r>
+                        <a:rPr lang="en-ID" sz="1400" i="1">
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        </a:rPr>
+                        <m:t>𝑥</m:t>
+                      </m:r>
+                      <m:r>
+                        <a:rPr lang="en-US" sz="1400" b="0" i="1">
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        </a:rPr>
+                        <m:t>|</m:t>
+                      </m:r>
+                    </m:e>
+                  </m:acc>
+                </m:oMath>
+              </a14:m>
+              <a:endParaRPr lang="en-ID" sz="1600"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2" name="TextBox 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA8E659C-447D-4EE3-9972-EFFCA70A3FCD}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3086098" y="566737"/>
+              <a:ext cx="1123952" cy="228589"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1400" b="0">
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>|</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1400" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑥−</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-ID" sz="1400" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>(𝑥</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1400" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>|</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-ID" sz="1400" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>) ̅</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-ID" sz="1600"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="981075" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1614,7 +1698,13 @@
       <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="4" name="TextBox 3"/>
+            <xdr:cNvPr id="4" name="TextBox 3">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000004000000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
             <xdr:cNvSpPr txBox="1"/>
           </xdr:nvSpPr>
           <xdr:spPr>
@@ -1763,7 +1853,13 @@
       <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="5" name="TextBox 4"/>
+            <xdr:cNvPr id="5" name="TextBox 4">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000005000000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
             <xdr:cNvSpPr txBox="1"/>
           </xdr:nvSpPr>
           <xdr:spPr>
@@ -1883,20 +1979,26 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>504825</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="987835" cy="250453"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="TextBox 5"/>
+        <xdr:cNvPr id="6" name="TextBox 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4772025" y="2409825"/>
+          <a:off x="7743825" y="2362200"/>
           <a:ext cx="987835" cy="250453"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1932,6 +2034,166 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1265026" cy="504825"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="7" name="TextBox 6">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{806CFA0A-8670-4DCE-A708-EF841D9F36D8}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="4686300" y="2390775"/>
+              <a:ext cx="1265026" cy="504825"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:noAutofit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:rad>
+                      <m:radPr>
+                        <m:degHide m:val="on"/>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1600" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:radPr>
+                      <m:deg/>
+                      <m:e>
+                        <m:eqArr>
+                          <m:eqArrPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-US" sz="1600" b="0" i="0">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:eqArrPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1600" b="0" i="0">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>548.007755</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:e/>
+                        </m:eqArr>
+                      </m:e>
+                    </m:rad>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="7" name="TextBox 6">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{806CFA0A-8670-4DCE-A708-EF841D9F36D8}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="4686300" y="2390775"/>
+              <a:ext cx="1265026" cy="504825"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:noAutofit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="en-US" sz="1600" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>√(</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1600" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>█(548.007755@))</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
 </xdr:wsDr>
@@ -2199,7 +2461,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2215,7 +2477,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="33" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
@@ -2223,7 +2485,7 @@
       </c>
     </row>
     <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="20"/>
+      <c r="A2" s="34"/>
       <c r="B2" s="8" t="s">
         <v>2</v>
       </c>
@@ -2868,11 +3130,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:R15"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="P14" sqref="P14"/>
+      <selection activeCell="M7" sqref="M7:N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3313,7 +3575,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A2:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3540,10 +3802,10 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="21" t="s">
+      <c r="A17" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="B17" s="21"/>
+      <c r="B17" s="35"/>
       <c r="C17" s="17" t="s">
         <v>45</v>
       </c>
@@ -3563,11 +3825,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B4:I13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3651,11 +3913,11 @@
         <f t="shared" si="1"/>
         <v>71.5</v>
       </c>
-      <c r="H7" s="22" t="s">
+      <c r="H7" s="19" t="s">
         <v>49</v>
       </c>
       <c r="I7" s="18">
-        <f>C12*(F12^2)/(C12-1)</f>
+        <f>(C12*(F12^2))/(C12-1)</f>
         <v>300312.5</v>
       </c>
     </row>
@@ -3770,11 +4032,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:I13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="B4:I15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="A1:XFD1048576"/>
+      <selection activeCell="F12" sqref="B4:F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3862,7 +4124,7 @@
         <v>47</v>
       </c>
       <c r="I7" s="2">
-        <f>C12*(F12^2)/(C12-1)</f>
+        <f>(C12*(F12^2))/(C12-1)</f>
         <v>300312.5</v>
       </c>
     </row>
@@ -3973,6 +4235,15 @@
     <row r="13" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="H13" s="18" t="s">
         <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="H15" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="I15" s="2">
+        <f>SQRT(548.0075)</f>
+        <v>23.409560012951975</v>
       </c>
     </row>
   </sheetData>
@@ -3982,15 +4253,487 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="B1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="9.85546875" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+    </row>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B3" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="G3" s="23"/>
+      <c r="H3" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="I3" s="26">
+        <f>1/4 *50</f>
+        <v>12.5</v>
+      </c>
+      <c r="J3" s="27" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B4" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="15">
+        <v>3</v>
+      </c>
+      <c r="D4" s="15">
+        <f>57-0.5</f>
+        <v>56.5</v>
+      </c>
+      <c r="E4" s="15">
+        <f>62+0.5</f>
+        <v>62.5</v>
+      </c>
+      <c r="F4" s="16">
+        <v>6</v>
+      </c>
+      <c r="H4" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="I4" s="26">
+        <f>3/4 *50</f>
+        <v>37.5</v>
+      </c>
+      <c r="J4" s="26" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B5" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="15">
+        <v>2</v>
+      </c>
+      <c r="D5" s="15">
+        <f>63-0.5</f>
+        <v>62.5</v>
+      </c>
+      <c r="E5" s="15">
+        <f>68+0.5</f>
+        <v>68.5</v>
+      </c>
+      <c r="F5" s="16">
+        <v>6</v>
+      </c>
+      <c r="H5" s="26"/>
+      <c r="I5" s="26"/>
+      <c r="J5" s="26"/>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="15">
+        <v>2</v>
+      </c>
+      <c r="D6" s="15">
+        <f>69-0.5</f>
+        <v>68.5</v>
+      </c>
+      <c r="E6" s="15">
+        <f>74+0.5</f>
+        <v>74.5</v>
+      </c>
+      <c r="F6" s="16">
+        <v>6</v>
+      </c>
+      <c r="H6" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="I6" s="28">
+        <f>D8+(((1/4*C11)-SUM(C4:C7))*F8)/C8</f>
+        <v>81.318181818181813</v>
+      </c>
+      <c r="J6" s="29"/>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B7" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="5">
+        <v>4</v>
+      </c>
+      <c r="D7" s="15">
+        <f>75-0.5</f>
+        <v>74.5</v>
+      </c>
+      <c r="E7" s="15">
+        <f>80+0.5</f>
+        <v>80.5</v>
+      </c>
+      <c r="F7" s="16">
+        <v>6</v>
+      </c>
+      <c r="H7" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="I7" s="30">
+        <f>D10+(((3/4*C11)-SUM(C4:C9))*F10)/C10</f>
+        <v>92.730769230769226</v>
+      </c>
+      <c r="J7" s="26"/>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B8" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="15">
+        <v>11</v>
+      </c>
+      <c r="D8" s="15">
+        <f>81-0.5</f>
+        <v>80.5</v>
+      </c>
+      <c r="E8" s="15">
+        <f>86+0.5</f>
+        <v>86.5</v>
+      </c>
+      <c r="F8" s="16">
+        <v>6</v>
+      </c>
+      <c r="H8" s="26"/>
+      <c r="I8" s="28"/>
+      <c r="J8" s="26"/>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B9" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" s="15">
+        <v>15</v>
+      </c>
+      <c r="D9" s="15">
+        <f>87-0.5</f>
+        <v>86.5</v>
+      </c>
+      <c r="E9" s="15">
+        <f>92+0.5</f>
+        <v>92.5</v>
+      </c>
+      <c r="F9" s="16">
+        <v>6</v>
+      </c>
+      <c r="H9" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="I9" s="28">
+        <f>1/2*(I7-I6)</f>
+        <v>5.7062937062937067</v>
+      </c>
+      <c r="J9" s="26"/>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" s="15">
+        <v>13</v>
+      </c>
+      <c r="D10" s="15">
+        <f>93-0.5</f>
+        <v>92.5</v>
+      </c>
+      <c r="E10" s="15">
+        <f>98+0.5</f>
+        <v>98.5</v>
+      </c>
+      <c r="F10" s="16">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="21">
+        <f>SUM(C4:C10)</f>
+        <v>50</v>
+      </c>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FE28418-80D4-49DA-B9F5-4C2B17E1683E}">
+  <dimension ref="B3:K11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="8" max="8" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B3" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="H3" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="I3" s="31">
+        <f>10/100*C11</f>
+        <v>5</v>
+      </c>
+      <c r="J3" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="K3" s="31"/>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B4" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="15">
+        <v>3</v>
+      </c>
+      <c r="D4" s="15">
+        <f>57-0.5</f>
+        <v>56.5</v>
+      </c>
+      <c r="E4" s="15">
+        <f>62+0.5</f>
+        <v>62.5</v>
+      </c>
+      <c r="F4" s="16">
+        <v>6</v>
+      </c>
+      <c r="H4" s="31" t="s">
+        <v>59</v>
+      </c>
+      <c r="I4" s="31">
+        <f>90/100*C11</f>
+        <v>45</v>
+      </c>
+      <c r="J4" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="K4" s="31"/>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B5" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="15">
+        <v>2</v>
+      </c>
+      <c r="D5" s="15">
+        <f>63-0.5</f>
+        <v>62.5</v>
+      </c>
+      <c r="E5" s="15">
+        <f>68+0.5</f>
+        <v>68.5</v>
+      </c>
+      <c r="F5" s="16">
+        <v>6</v>
+      </c>
+      <c r="H5" s="31"/>
+      <c r="I5" s="31"/>
+      <c r="J5" s="31"/>
+      <c r="K5" s="31"/>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B6" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="15">
+        <v>2</v>
+      </c>
+      <c r="D6" s="15">
+        <f>69-0.5</f>
+        <v>68.5</v>
+      </c>
+      <c r="E6" s="15">
+        <f>74+0.5</f>
+        <v>74.5</v>
+      </c>
+      <c r="F6" s="16">
+        <v>6</v>
+      </c>
+      <c r="H6" s="31" t="s">
+        <v>60</v>
+      </c>
+      <c r="I6" s="32">
+        <f>D5+(((10/100*C11)-C4)*F4)/C5</f>
+        <v>68.5</v>
+      </c>
+      <c r="J6" s="31"/>
+      <c r="K6" s="31"/>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B7" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="5">
+        <v>4</v>
+      </c>
+      <c r="D7" s="15">
+        <f>75-0.5</f>
+        <v>74.5</v>
+      </c>
+      <c r="E7" s="15">
+        <f>80+0.5</f>
+        <v>80.5</v>
+      </c>
+      <c r="F7" s="16">
+        <v>6</v>
+      </c>
+      <c r="H7" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="I7" s="32">
+        <f>D10+(((90/100*C11)-SUM(C4:C9))*F10)/C10</f>
+        <v>96.192307692307693</v>
+      </c>
+      <c r="J7" s="31"/>
+      <c r="K7" s="31"/>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B8" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="15">
+        <v>11</v>
+      </c>
+      <c r="D8" s="15">
+        <f>81-0.5</f>
+        <v>80.5</v>
+      </c>
+      <c r="E8" s="15">
+        <f>86+0.5</f>
+        <v>86.5</v>
+      </c>
+      <c r="F8" s="16">
+        <v>6</v>
+      </c>
+      <c r="H8" s="31"/>
+      <c r="I8" s="32"/>
+      <c r="J8" s="31"/>
+      <c r="K8" s="31"/>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B9" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" s="15">
+        <v>15</v>
+      </c>
+      <c r="D9" s="15">
+        <f>87-0.5</f>
+        <v>86.5</v>
+      </c>
+      <c r="E9" s="15">
+        <f>92+0.5</f>
+        <v>92.5</v>
+      </c>
+      <c r="F9" s="16">
+        <v>6</v>
+      </c>
+      <c r="H9" s="31" t="s">
+        <v>55</v>
+      </c>
+      <c r="I9" s="32">
+        <f>1/2*(I7-I6)</f>
+        <v>13.846153846153847</v>
+      </c>
+      <c r="J9" s="31"/>
+      <c r="K9" s="31"/>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B10" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" s="15">
+        <v>13</v>
+      </c>
+      <c r="D10" s="15">
+        <f>93-0.5</f>
+        <v>92.5</v>
+      </c>
+      <c r="E10" s="15">
+        <f>98+0.5</f>
+        <v>98.5</v>
+      </c>
+      <c r="F10" s="16">
+        <v>6</v>
+      </c>
+      <c r="H10" s="31"/>
+      <c r="I10" s="31"/>
+      <c r="J10" s="31"/>
+      <c r="K10" s="31"/>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B11" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="21">
+        <f>SUM(C4:C10)</f>
+        <v>50</v>
+      </c>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="2"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Perbaikan di excel, menggunakan metode data tunggal saja dan menyamakan hasil perhitungan dari rumus excel
</commit_message>
<xml_diff>
--- a/Data Penyebaran Data Frekuensi Tugas Kelompok.xlsx
+++ b/Data Penyebaran Data Frekuensi Tugas Kelompok.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hamdi\Documents\statistikafiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{569A81FC-58ED-4C46-996E-5FC0675AC8D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FA89E4B-CCAD-4344-8747-27F917D6A8D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="45" windowWidth="20490" windowHeight="10875" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="102">
   <si>
     <t>No. Urut</t>
   </si>
@@ -276,6 +276,120 @@
   <si>
     <t>Jumlah P90</t>
   </si>
+  <si>
+    <t>Jangkauan Kuartil</t>
+  </si>
+  <si>
+    <t>Kuartil adalah bilangan yang digunakan untuk membagi sekumpulan data menjadi 4 bagian yang jumlahnya sama banyak</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>Mean</t>
+  </si>
+  <si>
+    <t>Standard Error</t>
+  </si>
+  <si>
+    <t>Median</t>
+  </si>
+  <si>
+    <t>Mode</t>
+  </si>
+  <si>
+    <t>Standard Deviation</t>
+  </si>
+  <si>
+    <t>Sample Variance</t>
+  </si>
+  <si>
+    <t>Kurtosis</t>
+  </si>
+  <si>
+    <t>Skewness</t>
+  </si>
+  <si>
+    <t>Range</t>
+  </si>
+  <si>
+    <t>Minimum</t>
+  </si>
+  <si>
+    <t>Maximum</t>
+  </si>
+  <si>
+    <t>Sum</t>
+  </si>
+  <si>
+    <t>Count</t>
+  </si>
+  <si>
+    <t>Tidak terpakai</t>
+  </si>
+  <si>
+    <t>Rata-rata</t>
+  </si>
+  <si>
+    <t>|xi​−xˉ|</t>
+  </si>
+  <si>
+    <t>Hasil excel</t>
+  </si>
+  <si>
+    <t>Simpangan rata-rata jarak antara nilai-nilai data menuju rata-ratanya</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7 ,37 adalah rata-rata jumlah jarak nilai 50 siswa ke jumlah rata-rata nilai keseluruhan </t>
+  </si>
+  <si>
+    <t>(xi)^2</t>
+  </si>
+  <si>
+    <t>jumlah xi</t>
+  </si>
+  <si>
+    <t>jumlah xi^2</t>
+  </si>
+  <si>
+    <t>S^2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">s= </t>
+  </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>Q3</t>
+  </si>
+  <si>
+    <t>Nilai ke 38</t>
+  </si>
+  <si>
+    <t>Nilai ke 13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q2 = </t>
+  </si>
+  <si>
+    <t>Q2</t>
+  </si>
+  <si>
+    <t>Nilai ke 25</t>
+  </si>
+  <si>
+    <t>Rumus Excel</t>
+  </si>
+  <si>
+    <t>Kuartil bawah</t>
+  </si>
+  <si>
+    <t>median</t>
+  </si>
+  <si>
+    <t>Kuartil Atas</t>
+  </si>
 </sst>
 </file>
 
@@ -284,7 +398,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -375,8 +489,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -395,8 +517,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -465,6 +599,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -474,7 +628,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -554,6 +708,27 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="5" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="8" fillId="5" borderId="4" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1979,10 +2154,10 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="987835" cy="250453"/>
     <xdr:sp macro="" textlink="">
@@ -1998,7 +2173,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7743825" y="2362200"/>
+          <a:off x="4772025" y="2447925"/>
           <a:ext cx="987835" cy="250453"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2034,166 +2209,6 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="1265026" cy="504825"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="7" name="TextBox 6">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{806CFA0A-8670-4DCE-A708-EF841D9F36D8}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr txBox="1"/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="4686300" y="2390775"/>
-              <a:ext cx="1265026" cy="504825"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:lnRef>
-            <a:fillRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
-              <a:noAutofit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr/>
-              <a14:m>
-                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
-                  <m:oMathParaPr>
-                    <m:jc m:val="centerGroup"/>
-                  </m:oMathParaPr>
-                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
-                    <m:rad>
-                      <m:radPr>
-                        <m:degHide m:val="on"/>
-                        <m:ctrlPr>
-                          <a:rPr lang="en-US" sz="1600" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                        </m:ctrlPr>
-                      </m:radPr>
-                      <m:deg/>
-                      <m:e>
-                        <m:eqArr>
-                          <m:eqArrPr>
-                            <m:ctrlPr>
-                              <a:rPr lang="en-US" sz="1600" b="0" i="0">
-                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                              </a:rPr>
-                            </m:ctrlPr>
-                          </m:eqArrPr>
-                          <m:e>
-                            <m:r>
-                              <a:rPr lang="en-US" sz="1600" b="0" i="0">
-                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                              </a:rPr>
-                              <m:t>548.007755</m:t>
-                            </m:r>
-                          </m:e>
-                          <m:e/>
-                        </m:eqArr>
-                      </m:e>
-                    </m:rad>
-                  </m:oMath>
-                </m:oMathPara>
-              </a14:m>
-              <a:endParaRPr lang="en-US" sz="1100"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Choice>
-      <mc:Fallback>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="7" name="TextBox 6">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{806CFA0A-8670-4DCE-A708-EF841D9F36D8}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr txBox="1"/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="4686300" y="2390775"/>
-              <a:ext cx="1265026" cy="504825"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:lnRef>
-            <a:fillRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
-              <a:noAutofit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr/>
-              <a:r>
-                <a:rPr lang="en-US" sz="1600" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>√(</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-US" sz="1600" b="0" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>█(548.007755@))</a:t>
-              </a:r>
-              <a:endParaRPr lang="en-US" sz="1100"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Fallback>
-    </mc:AlternateContent>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
 </xdr:wsDr>
@@ -2464,8 +2479,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="G55" sqref="G55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2474,6 +2489,7 @@
     <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2949,7 +2965,7 @@
         <v>89.933333333333337</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>30</v>
       </c>
@@ -2957,7 +2973,7 @@
         <v>90.666666666666671</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
         <v>31</v>
       </c>
@@ -2965,7 +2981,7 @@
         <v>90.8</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="3">
         <v>32</v>
       </c>
@@ -2973,135 +2989,222 @@
         <v>90.866666666666674</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>33</v>
       </c>
       <c r="B36" s="5">
         <v>91.066666666666663</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="H36" s="38" t="s">
+        <v>66</v>
+      </c>
+      <c r="I36" s="38"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
         <v>34</v>
       </c>
       <c r="B37" s="5">
         <v>91.533333333333346</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H37" s="36"/>
+      <c r="I37" s="36"/>
+    </row>
+    <row r="38" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>35</v>
       </c>
       <c r="B38" s="5">
         <v>91.533333333333346</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H38" s="36" t="s">
+        <v>67</v>
+      </c>
+      <c r="I38" s="36">
+        <v>85.705333333333328</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>36</v>
       </c>
       <c r="B39" s="5">
         <v>92</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="H39" s="36" t="s">
+        <v>68</v>
+      </c>
+      <c r="I39" s="36">
+        <v>1.4179120928138926</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
         <v>37</v>
       </c>
       <c r="B40" s="5">
         <v>92.333333333333329</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H40" s="36" t="s">
+        <v>69</v>
+      </c>
+      <c r="I40" s="36">
+        <v>88.966666666666669</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>38</v>
       </c>
       <c r="B41" s="5">
         <v>92.733333333333334</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H41" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="I41" s="36">
+        <v>84.600000000000009</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>39</v>
       </c>
       <c r="B42" s="5">
         <v>92.933333333333337</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="H42" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="I42" s="36">
+        <v>10.026152559551129</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
         <v>40</v>
       </c>
       <c r="B43" s="5">
         <v>93.2</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H43" s="36" t="s">
+        <v>72</v>
+      </c>
+      <c r="I43" s="36">
+        <v>100.52373514739364</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>41</v>
       </c>
       <c r="B44" s="5">
         <v>94</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H44" s="36" t="s">
+        <v>73</v>
+      </c>
+      <c r="I44" s="36">
+        <v>1.4547799557831986</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>42</v>
       </c>
       <c r="B45" s="5">
         <v>94.066666666666663</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="H45" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="I45" s="36">
+        <v>-1.44069540750446</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
         <v>43</v>
       </c>
       <c r="B46" s="5">
         <v>94.133333333333326</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H46" s="36" t="s">
+        <v>75</v>
+      </c>
+      <c r="I46" s="36">
+        <v>40.066666666666663</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>44</v>
       </c>
       <c r="B47" s="5">
         <v>94.600000000000009</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H47" s="36" t="s">
+        <v>76</v>
+      </c>
+      <c r="I47" s="36">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>45</v>
       </c>
       <c r="B48" s="5">
         <v>94.866666666666674</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="H48" s="36" t="s">
+        <v>77</v>
+      </c>
+      <c r="I48" s="36">
+        <v>97.066666666666663</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="4">
         <v>46</v>
       </c>
       <c r="B49" s="5">
         <v>95.066666666666663</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H49" s="36" t="s">
+        <v>78</v>
+      </c>
+      <c r="I49" s="36">
+        <v>4285.2666666666664</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="3">
         <v>47</v>
       </c>
       <c r="B50" s="6">
         <v>95.666666666666671</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H50" s="37" t="s">
+        <v>79</v>
+      </c>
+      <c r="I50" s="37">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
         <v>48</v>
       </c>
       <c r="B51" s="6">
         <v>95.666666666666671</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="I51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="4">
         <v>49</v>
       </c>
@@ -3109,7 +3212,7 @@
         <v>96.466666666666654</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
         <v>50</v>
       </c>
@@ -3131,10 +3234,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B1:R15"/>
+  <dimension ref="B1:S17"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7:N15"/>
+      <selection activeCell="R3" sqref="R3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3143,15 +3246,21 @@
     <col min="14" max="14" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>28</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="39" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="2" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="N1" s="39"/>
+      <c r="O1" s="39"/>
+      <c r="P1" s="39"/>
+      <c r="Q1" s="39"/>
+      <c r="R1" s="39"/>
+      <c r="S1" s="39"/>
+    </row>
+    <row r="2" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B2" s="5">
         <v>90.8</v>
       </c>
@@ -3182,11 +3291,17 @@
       <c r="K2" s="5">
         <v>93.2</v>
       </c>
-      <c r="M2" t="s">
+      <c r="M2" s="39" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="3" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="N2" s="39"/>
+      <c r="O2" s="39"/>
+      <c r="P2" s="39"/>
+      <c r="Q2" s="39"/>
+      <c r="R2" s="39"/>
+      <c r="S2" s="39"/>
+    </row>
+    <row r="3" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B3" s="5">
         <v>86.333333333333329</v>
       </c>
@@ -3217,19 +3332,23 @@
       <c r="K3" s="5">
         <v>90.666666666666671</v>
       </c>
-      <c r="M3" t="s">
+      <c r="M3" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="Q3">
+      <c r="N3" s="39"/>
+      <c r="O3" s="39"/>
+      <c r="P3" s="39"/>
+      <c r="Q3" s="39">
         <f xml:space="preserve"> 1+ 3.3 * LOG(50)</f>
         <v>6.6066010143088612</v>
       </c>
-      <c r="R3" s="13">
+      <c r="R3" s="40">
         <f>Q3</f>
         <v>6.6066010143088612</v>
       </c>
-    </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="S3" s="39"/>
+    </row>
+    <row r="4" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B4" s="6">
         <v>80</v>
       </c>
@@ -3260,15 +3379,20 @@
       <c r="K4" s="5">
         <v>86.133333333333326</v>
       </c>
-      <c r="M4" t="s">
+      <c r="M4" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="Q4" s="13">
+      <c r="N4" s="39"/>
+      <c r="O4" s="39"/>
+      <c r="P4" s="39"/>
+      <c r="Q4" s="40">
         <f>K14-B10</f>
         <v>40.066666666666663</v>
       </c>
-    </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="R4" s="39"/>
+      <c r="S4" s="39"/>
+    </row>
+    <row r="5" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B5" s="5">
         <v>94</v>
       </c>
@@ -3299,19 +3423,23 @@
       <c r="K5" s="5">
         <v>97.066666666666663</v>
       </c>
-      <c r="M5" t="s">
+      <c r="M5" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="Q5">
+      <c r="N5" s="39"/>
+      <c r="O5" s="39"/>
+      <c r="P5" s="39"/>
+      <c r="Q5" s="39">
         <f>Q4/R3</f>
         <v>6.0646414971766189</v>
       </c>
-      <c r="R5" s="13">
+      <c r="R5" s="40">
         <f>Q5</f>
         <v>6.0646414971766189</v>
       </c>
-    </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="S5" s="39"/>
+    </row>
+    <row r="6" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B6" s="6">
         <v>57</v>
       </c>
@@ -3342,35 +3470,57 @@
       <c r="K6" s="6">
         <v>79.666666666666671</v>
       </c>
-    </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="M7" s="15" t="s">
+      <c r="M6" s="39"/>
+      <c r="N6" s="39"/>
+      <c r="O6" s="39"/>
+      <c r="P6" s="39"/>
+      <c r="Q6" s="39"/>
+      <c r="R6" s="39"/>
+      <c r="S6" s="39"/>
+    </row>
+    <row r="7" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="M7" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="N7" s="15" t="s">
+      <c r="N7" s="41" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="M8" s="15" t="s">
+      <c r="O7" s="39"/>
+      <c r="P7" s="39"/>
+      <c r="Q7" s="39"/>
+      <c r="R7" s="39"/>
+      <c r="S7" s="39"/>
+    </row>
+    <row r="8" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="M8" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="N8" s="15">
+      <c r="N8" s="41">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="O8" s="39"/>
+      <c r="P8" s="39"/>
+      <c r="Q8" s="39"/>
+      <c r="R8" s="39"/>
+      <c r="S8" s="39"/>
+    </row>
+    <row r="9" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>27</v>
       </c>
-      <c r="M9" s="15" t="s">
+      <c r="M9" s="41" t="s">
         <v>37</v>
       </c>
-      <c r="N9" s="15">
+      <c r="N9" s="41">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="O9" s="39"/>
+      <c r="P9" s="39"/>
+      <c r="Q9" s="39"/>
+      <c r="R9" s="39"/>
+      <c r="S9" s="39"/>
+    </row>
+    <row r="10" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B10" s="6">
         <v>57</v>
       </c>
@@ -3401,14 +3551,19 @@
       <c r="K10" s="6">
         <v>79.666666666666671</v>
       </c>
-      <c r="M10" s="15" t="s">
+      <c r="M10" s="41" t="s">
         <v>38</v>
       </c>
-      <c r="N10" s="15">
+      <c r="N10" s="41">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="O10" s="39"/>
+      <c r="P10" s="39"/>
+      <c r="Q10" s="39"/>
+      <c r="R10" s="39"/>
+      <c r="S10" s="39"/>
+    </row>
+    <row r="11" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B11" s="6">
         <v>80</v>
       </c>
@@ -3439,14 +3594,19 @@
       <c r="K11" s="5">
         <v>86.133333333333326</v>
       </c>
-      <c r="M11" s="15" t="s">
+      <c r="M11" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="N11" s="5">
+      <c r="N11" s="42">
         <v>4</v>
       </c>
-    </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="O11" s="39"/>
+      <c r="P11" s="39"/>
+      <c r="Q11" s="39"/>
+      <c r="R11" s="39"/>
+      <c r="S11" s="39"/>
+    </row>
+    <row r="12" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B12" s="5">
         <v>86.333333333333329</v>
       </c>
@@ -3477,14 +3637,19 @@
       <c r="K12" s="5">
         <v>90.666666666666671</v>
       </c>
-      <c r="M12" s="15" t="s">
+      <c r="M12" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="N12" s="15">
+      <c r="N12" s="41">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="O12" s="39"/>
+      <c r="P12" s="39"/>
+      <c r="Q12" s="39"/>
+      <c r="R12" s="39"/>
+      <c r="S12" s="39"/>
+    </row>
+    <row r="13" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B13" s="5">
         <v>90.8</v>
       </c>
@@ -3515,14 +3680,19 @@
       <c r="K13" s="5">
         <v>93.2</v>
       </c>
-      <c r="M13" s="15" t="s">
+      <c r="M13" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="N13" s="15">
+      <c r="N13" s="41">
         <v>15</v>
       </c>
-    </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="O13" s="39"/>
+      <c r="P13" s="39"/>
+      <c r="Q13" s="39"/>
+      <c r="R13" s="39"/>
+      <c r="S13" s="39"/>
+    </row>
+    <row r="14" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B14" s="5">
         <v>94</v>
       </c>
@@ -3553,20 +3723,36 @@
       <c r="K14" s="5">
         <v>97.066666666666663</v>
       </c>
-      <c r="M14" s="15" t="s">
+      <c r="M14" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="N14" s="15">
+      <c r="N14" s="41">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="M15" s="15" t="s">
+      <c r="O14" s="39"/>
+      <c r="P14" s="39"/>
+      <c r="Q14" s="39"/>
+      <c r="R14" s="39"/>
+      <c r="S14" s="39"/>
+    </row>
+    <row r="15" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="M15" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="N15" s="15">
+      <c r="N15" s="41">
         <f>SUM(N8:N14)</f>
         <v>50</v>
+      </c>
+      <c r="O15" s="39"/>
+      <c r="P15" s="39"/>
+      <c r="Q15" s="39"/>
+      <c r="R15" s="39"/>
+      <c r="S15" s="39"/>
+    </row>
+    <row r="17" spans="14:15" x14ac:dyDescent="0.25">
+      <c r="N17" s="39"/>
+      <c r="O17" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -3576,10 +3762,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A2:G17"/>
+  <dimension ref="A2:R54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5:L54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3587,12 +3773,41 @@
     <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.42578125" customWidth="1"/>
     <col min="7" max="7" width="14.28515625" customWidth="1"/>
+    <col min="13" max="13" width="21.140625" style="43" customWidth="1"/>
+    <col min="16" max="16" width="9.140625" style="43"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M2" s="43"/>
+      <c r="P2" s="43"/>
+      <c r="R2" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="2:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M3" s="43">
+        <f>SUM(L5:L54)/50</f>
+        <v>85.705333333333328</v>
+      </c>
+      <c r="N3" t="s">
+        <v>81</v>
+      </c>
+      <c r="P3" s="43">
+        <f>SUM(M5:M54)/50</f>
+        <v>7.3729600000000017</v>
+      </c>
+      <c r="R3" s="2">
+        <f>AVEDEV(L5:L54)</f>
+        <v>7.3729600000000017</v>
+      </c>
+    </row>
+    <row r="4" spans="2:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M4" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="P4" s="43"/>
+    </row>
+    <row r="5" spans="2:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="15" t="s">
         <v>34</v>
       </c>
@@ -3607,8 +3822,15 @@
       </c>
       <c r="F5" s="16"/>
       <c r="G5" s="16"/>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="L5" s="6">
+        <v>57</v>
+      </c>
+      <c r="M5" s="43">
+        <f>ABS(L5-$M$3)</f>
+        <v>28.705333333333328</v>
+      </c>
+    </row>
+    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B6" s="15" t="s">
         <v>36</v>
       </c>
@@ -3631,8 +3853,15 @@
         <f>C6*F6</f>
         <v>77.399999999999991</v>
       </c>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="L6" s="5">
+        <v>60</v>
+      </c>
+      <c r="M6" s="43">
+        <f t="shared" ref="M6:M54" si="0">ABS(L6-$M$3)</f>
+        <v>25.705333333333328</v>
+      </c>
+    </row>
+    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B7" s="15" t="s">
         <v>37</v>
       </c>
@@ -3644,19 +3873,26 @@
         <v>65.5</v>
       </c>
       <c r="E7" s="16">
-        <f t="shared" ref="E7:E12" si="0">C7*D7</f>
+        <f t="shared" ref="E7:E12" si="1">C7*D7</f>
         <v>131</v>
       </c>
       <c r="F7" s="16">
-        <f t="shared" ref="F7:F12" si="1">(ABS(D7-$D$16))</f>
+        <f t="shared" ref="F7:F12" si="2">(ABS(D7-$D$16))</f>
         <v>19.799999999999997</v>
       </c>
       <c r="G7" s="16">
-        <f t="shared" ref="G7:G12" si="2">C7*F7</f>
+        <f t="shared" ref="G7:G12" si="3">C7*F7</f>
         <v>39.599999999999994</v>
       </c>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="L7" s="5">
+        <v>62</v>
+      </c>
+      <c r="M7" s="43">
+        <f t="shared" si="0"/>
+        <v>23.705333333333328</v>
+      </c>
+    </row>
+    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B8" s="15" t="s">
         <v>38</v>
       </c>
@@ -3668,19 +3904,26 @@
         <v>71.5</v>
       </c>
       <c r="E8" s="16">
+        <f t="shared" si="1"/>
+        <v>143</v>
+      </c>
+      <c r="F8" s="16">
+        <f t="shared" si="2"/>
+        <v>13.799999999999997</v>
+      </c>
+      <c r="G8" s="16">
+        <f t="shared" si="3"/>
+        <v>27.599999999999994</v>
+      </c>
+      <c r="L8" s="5">
+        <v>63.066666666666663</v>
+      </c>
+      <c r="M8" s="43">
         <f t="shared" si="0"/>
-        <v>143</v>
-      </c>
-      <c r="F8" s="16">
-        <f t="shared" si="1"/>
-        <v>13.799999999999997</v>
-      </c>
-      <c r="G8" s="16">
-        <f t="shared" si="2"/>
-        <v>27.599999999999994</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+        <v>22.638666666666666</v>
+      </c>
+    </row>
+    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B9" s="15" t="s">
         <v>39</v>
       </c>
@@ -3692,19 +3935,26 @@
         <v>77.5</v>
       </c>
       <c r="E9" s="16">
+        <f t="shared" si="1"/>
+        <v>310</v>
+      </c>
+      <c r="F9" s="16">
+        <f t="shared" si="2"/>
+        <v>7.7999999999999972</v>
+      </c>
+      <c r="G9" s="16">
+        <f t="shared" si="3"/>
+        <v>31.199999999999989</v>
+      </c>
+      <c r="L9" s="6">
+        <v>66</v>
+      </c>
+      <c r="M9" s="43">
         <f t="shared" si="0"/>
-        <v>310</v>
-      </c>
-      <c r="F9" s="16">
-        <f t="shared" si="1"/>
-        <v>7.7999999999999972</v>
-      </c>
-      <c r="G9" s="16">
-        <f t="shared" si="2"/>
-        <v>31.199999999999989</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+        <v>19.705333333333328</v>
+      </c>
+    </row>
+    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B10" s="15" t="s">
         <v>40</v>
       </c>
@@ -3716,19 +3966,26 @@
         <v>83.5</v>
       </c>
       <c r="E10" s="16">
+        <f t="shared" si="1"/>
+        <v>918.5</v>
+      </c>
+      <c r="F10" s="16">
+        <f t="shared" si="2"/>
+        <v>1.7999999999999972</v>
+      </c>
+      <c r="G10" s="16">
+        <f t="shared" si="3"/>
+        <v>19.799999999999969</v>
+      </c>
+      <c r="L10" s="6">
+        <v>70</v>
+      </c>
+      <c r="M10" s="43">
         <f t="shared" si="0"/>
-        <v>918.5</v>
-      </c>
-      <c r="F10" s="16">
-        <f t="shared" si="1"/>
-        <v>1.7999999999999972</v>
-      </c>
-      <c r="G10" s="16">
-        <f t="shared" si="2"/>
-        <v>19.799999999999969</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+        <v>15.705333333333328</v>
+      </c>
+    </row>
+    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B11" s="15" t="s">
         <v>41</v>
       </c>
@@ -3740,19 +3997,26 @@
         <v>89.5</v>
       </c>
       <c r="E11" s="16">
+        <f t="shared" si="1"/>
+        <v>1342.5</v>
+      </c>
+      <c r="F11" s="16">
+        <f t="shared" si="2"/>
+        <v>4.2000000000000028</v>
+      </c>
+      <c r="G11" s="16">
+        <f t="shared" si="3"/>
+        <v>63.000000000000043</v>
+      </c>
+      <c r="L11" s="6">
+        <v>74</v>
+      </c>
+      <c r="M11" s="43">
         <f t="shared" si="0"/>
-        <v>1342.5</v>
-      </c>
-      <c r="F11" s="16">
-        <f t="shared" si="1"/>
-        <v>4.2000000000000028</v>
-      </c>
-      <c r="G11" s="16">
-        <f t="shared" si="2"/>
-        <v>63.000000000000043</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+        <v>11.705333333333328</v>
+      </c>
+    </row>
+    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B12" s="15" t="s">
         <v>42</v>
       </c>
@@ -3764,19 +4028,26 @@
         <v>95.5</v>
       </c>
       <c r="E12" s="16">
+        <f t="shared" si="1"/>
+        <v>1241.5</v>
+      </c>
+      <c r="F12" s="16">
+        <f t="shared" si="2"/>
+        <v>10.200000000000003</v>
+      </c>
+      <c r="G12" s="16">
+        <f t="shared" si="3"/>
+        <v>132.60000000000002</v>
+      </c>
+      <c r="L12" s="6">
+        <v>78</v>
+      </c>
+      <c r="M12" s="43">
         <f t="shared" si="0"/>
-        <v>1241.5</v>
-      </c>
-      <c r="F12" s="16">
-        <f t="shared" si="1"/>
-        <v>10.200000000000003</v>
-      </c>
-      <c r="G12" s="16">
-        <f t="shared" si="2"/>
-        <v>132.60000000000002</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+        <v>7.7053333333333285</v>
+      </c>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B13" s="15" t="s">
         <v>14</v>
       </c>
@@ -3794,14 +4065,46 @@
         <f>SUM(G6:G12)</f>
         <v>391.2</v>
       </c>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="L13" s="5">
+        <v>79.466666666666669</v>
+      </c>
+      <c r="M13" s="43">
+        <f t="shared" si="0"/>
+        <v>6.2386666666666599</v>
+      </c>
+    </row>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="L14" s="6">
+        <v>79.666666666666671</v>
+      </c>
+      <c r="M14" s="43">
+        <f t="shared" si="0"/>
+        <v>6.0386666666666571</v>
+      </c>
+    </row>
+    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="L15" s="6">
+        <v>80</v>
+      </c>
+      <c r="M15" s="43">
+        <f t="shared" si="0"/>
+        <v>5.7053333333333285</v>
+      </c>
+    </row>
+    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
       <c r="D16">
         <f>E13/C13</f>
         <v>85.3</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="L16" s="6">
+        <v>80.666666666666671</v>
+      </c>
+      <c r="M16" s="43">
+        <f t="shared" si="0"/>
+        <v>5.0386666666666571</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="35" t="s">
         <v>46</v>
       </c>
@@ -3812,6 +4115,352 @@
       <c r="D17">
         <f>G13/C13</f>
         <v>7.8239999999999998</v>
+      </c>
+      <c r="L17" s="5">
+        <v>83.533333333333331</v>
+      </c>
+      <c r="M17" s="43">
+        <f t="shared" si="0"/>
+        <v>2.171999999999997</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E18" t="s">
+        <v>84</v>
+      </c>
+      <c r="L18" s="5">
+        <v>84.399999999999991</v>
+      </c>
+      <c r="M18" s="43">
+        <f t="shared" si="0"/>
+        <v>1.305333333333337</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>85</v>
+      </c>
+      <c r="L19" s="5">
+        <v>84.600000000000009</v>
+      </c>
+      <c r="M19" s="43">
+        <f t="shared" si="0"/>
+        <v>1.10533333333332</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L20" s="5">
+        <v>84.600000000000009</v>
+      </c>
+      <c r="M20" s="43">
+        <f t="shared" si="0"/>
+        <v>1.10533333333332</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L21" s="6">
+        <v>85.666666666666671</v>
+      </c>
+      <c r="M21" s="43">
+        <f t="shared" si="0"/>
+        <v>3.8666666666657079E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L22" s="5">
+        <v>85.733333333333334</v>
+      </c>
+      <c r="M22" s="43">
+        <f t="shared" si="0"/>
+        <v>2.8000000000005798E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L23" s="5">
+        <v>86</v>
+      </c>
+      <c r="M23" s="43">
+        <f t="shared" si="0"/>
+        <v>0.29466666666667152</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L24" s="5">
+        <v>86.133333333333326</v>
+      </c>
+      <c r="M24" s="43">
+        <f t="shared" si="0"/>
+        <v>0.42799999999999727</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L25" s="5">
+        <v>86.333333333333329</v>
+      </c>
+      <c r="M25" s="43">
+        <f t="shared" si="0"/>
+        <v>0.62800000000000011</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L26" s="6">
+        <v>86.333333333333329</v>
+      </c>
+      <c r="M26" s="43">
+        <f t="shared" si="0"/>
+        <v>0.62800000000000011</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L27" s="5">
+        <v>86.666666666666671</v>
+      </c>
+      <c r="M27" s="43">
+        <f t="shared" si="0"/>
+        <v>0.96133333333334292</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L28" s="6">
+        <v>87</v>
+      </c>
+      <c r="M28" s="43">
+        <f t="shared" si="0"/>
+        <v>1.2946666666666715</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L29" s="6">
+        <v>88.666666666666671</v>
+      </c>
+      <c r="M29" s="43">
+        <f t="shared" si="0"/>
+        <v>2.9613333333333429</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L30" s="5">
+        <v>89.266666666666666</v>
+      </c>
+      <c r="M30" s="43">
+        <f t="shared" si="0"/>
+        <v>3.5613333333333372</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L31" s="5">
+        <v>89.466666666666654</v>
+      </c>
+      <c r="M31" s="43">
+        <f t="shared" si="0"/>
+        <v>3.7613333333333259</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L32" s="5">
+        <v>89.8</v>
+      </c>
+      <c r="M32" s="43">
+        <f t="shared" si="0"/>
+        <v>4.0946666666666687</v>
+      </c>
+    </row>
+    <row r="33" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L33" s="5">
+        <v>89.933333333333337</v>
+      </c>
+      <c r="M33" s="43">
+        <f t="shared" si="0"/>
+        <v>4.2280000000000086</v>
+      </c>
+    </row>
+    <row r="34" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L34" s="5">
+        <v>90.666666666666671</v>
+      </c>
+      <c r="M34" s="43">
+        <f t="shared" si="0"/>
+        <v>4.9613333333333429</v>
+      </c>
+    </row>
+    <row r="35" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L35" s="5">
+        <v>90.8</v>
+      </c>
+      <c r="M35" s="43">
+        <f t="shared" si="0"/>
+        <v>5.0946666666666687</v>
+      </c>
+    </row>
+    <row r="36" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L36" s="5">
+        <v>90.866666666666674</v>
+      </c>
+      <c r="M36" s="43">
+        <f t="shared" si="0"/>
+        <v>5.1613333333333458</v>
+      </c>
+    </row>
+    <row r="37" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L37" s="5">
+        <v>91.066666666666663</v>
+      </c>
+      <c r="M37" s="43">
+        <f t="shared" si="0"/>
+        <v>5.3613333333333344</v>
+      </c>
+    </row>
+    <row r="38" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L38" s="5">
+        <v>91.533333333333346</v>
+      </c>
+      <c r="M38" s="43">
+        <f t="shared" si="0"/>
+        <v>5.8280000000000172</v>
+      </c>
+    </row>
+    <row r="39" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L39" s="5">
+        <v>91.533333333333346</v>
+      </c>
+      <c r="M39" s="43">
+        <f t="shared" si="0"/>
+        <v>5.8280000000000172</v>
+      </c>
+    </row>
+    <row r="40" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L40" s="5">
+        <v>92</v>
+      </c>
+      <c r="M40" s="43">
+        <f t="shared" si="0"/>
+        <v>6.2946666666666715</v>
+      </c>
+    </row>
+    <row r="41" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L41" s="5">
+        <v>92.333333333333329</v>
+      </c>
+      <c r="M41" s="43">
+        <f t="shared" si="0"/>
+        <v>6.6280000000000001</v>
+      </c>
+    </row>
+    <row r="42" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L42" s="5">
+        <v>92.733333333333334</v>
+      </c>
+      <c r="M42" s="43">
+        <f t="shared" si="0"/>
+        <v>7.0280000000000058</v>
+      </c>
+    </row>
+    <row r="43" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L43" s="5">
+        <v>92.933333333333337</v>
+      </c>
+      <c r="M43" s="43">
+        <f t="shared" si="0"/>
+        <v>7.2280000000000086</v>
+      </c>
+    </row>
+    <row r="44" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L44" s="5">
+        <v>93.2</v>
+      </c>
+      <c r="M44" s="43">
+        <f t="shared" si="0"/>
+        <v>7.4946666666666744</v>
+      </c>
+    </row>
+    <row r="45" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L45" s="5">
+        <v>94</v>
+      </c>
+      <c r="M45" s="43">
+        <f t="shared" si="0"/>
+        <v>8.2946666666666715</v>
+      </c>
+    </row>
+    <row r="46" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L46" s="5">
+        <v>94.066666666666663</v>
+      </c>
+      <c r="M46" s="43">
+        <f t="shared" si="0"/>
+        <v>8.3613333333333344</v>
+      </c>
+    </row>
+    <row r="47" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L47" s="5">
+        <v>94.133333333333326</v>
+      </c>
+      <c r="M47" s="43">
+        <f t="shared" si="0"/>
+        <v>8.4279999999999973</v>
+      </c>
+    </row>
+    <row r="48" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L48" s="5">
+        <v>94.600000000000009</v>
+      </c>
+      <c r="M48" s="43">
+        <f t="shared" si="0"/>
+        <v>8.89466666666668</v>
+      </c>
+    </row>
+    <row r="49" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L49" s="5">
+        <v>94.866666666666674</v>
+      </c>
+      <c r="M49" s="43">
+        <f t="shared" si="0"/>
+        <v>9.1613333333333458</v>
+      </c>
+    </row>
+    <row r="50" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L50" s="5">
+        <v>95.066666666666663</v>
+      </c>
+      <c r="M50" s="43">
+        <f t="shared" si="0"/>
+        <v>9.3613333333333344</v>
+      </c>
+    </row>
+    <row r="51" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L51" s="6">
+        <v>95.666666666666671</v>
+      </c>
+      <c r="M51" s="43">
+        <f t="shared" si="0"/>
+        <v>9.9613333333333429</v>
+      </c>
+    </row>
+    <row r="52" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L52" s="6">
+        <v>95.666666666666671</v>
+      </c>
+      <c r="M52" s="43">
+        <f t="shared" si="0"/>
+        <v>9.9613333333333429</v>
+      </c>
+    </row>
+    <row r="53" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L53" s="5">
+        <v>96.466666666666654</v>
+      </c>
+      <c r="M53" s="43">
+        <f t="shared" si="0"/>
+        <v>10.761333333333326</v>
+      </c>
+    </row>
+    <row r="54" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L54" s="5">
+        <v>97.066666666666663</v>
+      </c>
+      <c r="M54" s="43">
+        <f t="shared" si="0"/>
+        <v>11.361333333333334</v>
       </c>
     </row>
   </sheetData>
@@ -3826,10 +4475,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="B4:I13"/>
+  <dimension ref="B3:R53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="N4" sqref="N4:N53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3839,7 +4488,18 @@
     <col min="10" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="O3" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B4" s="15" t="s">
         <v>34</v>
       </c>
@@ -3853,8 +4513,27 @@
         <v>44</v>
       </c>
       <c r="F4" s="16"/>
-    </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="N4" s="6">
+        <v>57</v>
+      </c>
+      <c r="O4" s="13">
+        <f>SUM(N4:N53)</f>
+        <v>4285.2666666666664</v>
+      </c>
+      <c r="P4" s="13">
+        <f>N4^2</f>
+        <v>3249</v>
+      </c>
+      <c r="Q4" s="13">
+        <f>SUM(P4:P53)</f>
+        <v>372195.87111111113</v>
+      </c>
+      <c r="R4" s="13">
+        <f>O4^2</f>
+        <v>18363510.404444441</v>
+      </c>
+    </row>
+    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B5" s="15" t="s">
         <v>36</v>
       </c>
@@ -3873,8 +4552,15 @@
         <f>(ABS(D5-$D$16))</f>
         <v>59.5</v>
       </c>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="N5" s="5">
+        <v>60</v>
+      </c>
+      <c r="P5" s="13">
+        <f>N5^2</f>
+        <v>3600</v>
+      </c>
+    </row>
+    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B6" s="15" t="s">
         <v>37</v>
       </c>
@@ -3893,8 +4579,15 @@
         <f t="shared" ref="F6:F11" si="1">(ABS(D6-$D$16))</f>
         <v>65.5</v>
       </c>
-    </row>
-    <row r="7" spans="2:9" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="N6" s="5">
+        <v>62</v>
+      </c>
+      <c r="P6" s="13">
+        <f>N6^2</f>
+        <v>3844</v>
+      </c>
+    </row>
+    <row r="7" spans="2:18" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B7" s="15" t="s">
         <v>38</v>
       </c>
@@ -3920,8 +4613,15 @@
         <f>(C12*(F12^2))/(C12-1)</f>
         <v>300312.5</v>
       </c>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="N7" s="5">
+        <v>63.066666666666663</v>
+      </c>
+      <c r="P7" s="13">
+        <f>N7^2</f>
+        <v>3977.4044444444439</v>
+      </c>
+    </row>
+    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B8" s="15" t="s">
         <v>39</v>
       </c>
@@ -3940,8 +4640,15 @@
         <f t="shared" si="1"/>
         <v>77.5</v>
       </c>
-    </row>
-    <row r="9" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="N8" s="6">
+        <v>66</v>
+      </c>
+      <c r="P8" s="13">
+        <f>N8^2</f>
+        <v>4356</v>
+      </c>
+    </row>
+    <row r="9" spans="2:18" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B9" s="15" t="s">
         <v>40</v>
       </c>
@@ -3960,9 +4667,22 @@
         <f t="shared" si="1"/>
         <v>83.5</v>
       </c>
-      <c r="H9" s="18"/>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H9" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="I9" s="2">
+        <f>((50*Variansi!Q4)-Variansi!R4)/(50*49)</f>
+        <v>100.52373514739378</v>
+      </c>
+      <c r="N9" s="6">
+        <v>70</v>
+      </c>
+      <c r="P9" s="13">
+        <f>N9^2</f>
+        <v>4900</v>
+      </c>
+    </row>
+    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B10" s="15" t="s">
         <v>41</v>
       </c>
@@ -3981,8 +4701,15 @@
         <f t="shared" si="1"/>
         <v>89.5</v>
       </c>
-    </row>
-    <row r="11" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="N10" s="6">
+        <v>74</v>
+      </c>
+      <c r="P10" s="13">
+        <f>N10^2</f>
+        <v>5476</v>
+      </c>
+    </row>
+    <row r="11" spans="2:18" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B11" s="15" t="s">
         <v>42</v>
       </c>
@@ -4001,9 +4728,22 @@
         <f t="shared" si="1"/>
         <v>95.5</v>
       </c>
-      <c r="H11" s="18"/>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H11" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="I11" s="2">
+        <f>SQRT(I9)</f>
+        <v>10.026152559551136</v>
+      </c>
+      <c r="N11" s="6">
+        <v>78</v>
+      </c>
+      <c r="P11" s="13">
+        <f>N11^2</f>
+        <v>6084</v>
+      </c>
+    </row>
+    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B12" s="15" t="s">
         <v>14</v>
       </c>
@@ -4020,9 +4760,383 @@
         <f>SUM(F5:F11)</f>
         <v>542.5</v>
       </c>
-    </row>
-    <row r="13" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="N12" s="5">
+        <v>79.466666666666669</v>
+      </c>
+      <c r="P12" s="13">
+        <f>N12^2</f>
+        <v>6314.9511111111115</v>
+      </c>
+    </row>
+    <row r="13" spans="2:18" ht="18.75" x14ac:dyDescent="0.3">
       <c r="H13" s="18"/>
+      <c r="N13" s="6">
+        <v>79.666666666666671</v>
+      </c>
+      <c r="P13" s="13">
+        <f>N13^2</f>
+        <v>6346.7777777777783</v>
+      </c>
+    </row>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="N14" s="6">
+        <v>80</v>
+      </c>
+      <c r="P14" s="13">
+        <f>N14^2</f>
+        <v>6400</v>
+      </c>
+    </row>
+    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="N15" s="6">
+        <v>80.666666666666671</v>
+      </c>
+      <c r="P15" s="13">
+        <f>N15^2</f>
+        <v>6507.1111111111122</v>
+      </c>
+    </row>
+    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="N16" s="5">
+        <v>83.533333333333331</v>
+      </c>
+      <c r="P16" s="13">
+        <f>N16^2</f>
+        <v>6977.8177777777773</v>
+      </c>
+    </row>
+    <row r="17" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N17" s="5">
+        <v>84.399999999999991</v>
+      </c>
+      <c r="P17" s="13">
+        <f>N17^2</f>
+        <v>7123.3599999999988</v>
+      </c>
+    </row>
+    <row r="18" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N18" s="5">
+        <v>84.600000000000009</v>
+      </c>
+      <c r="P18" s="13">
+        <f>N18^2</f>
+        <v>7157.1600000000017</v>
+      </c>
+    </row>
+    <row r="19" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N19" s="5">
+        <v>84.600000000000009</v>
+      </c>
+      <c r="P19" s="13">
+        <f>N19^2</f>
+        <v>7157.1600000000017</v>
+      </c>
+    </row>
+    <row r="20" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N20" s="6">
+        <v>85.666666666666671</v>
+      </c>
+      <c r="P20" s="13">
+        <f>N20^2</f>
+        <v>7338.7777777777783</v>
+      </c>
+    </row>
+    <row r="21" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N21" s="5">
+        <v>85.733333333333334</v>
+      </c>
+      <c r="P21" s="13">
+        <f>N21^2</f>
+        <v>7350.2044444444446</v>
+      </c>
+    </row>
+    <row r="22" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N22" s="5">
+        <v>86</v>
+      </c>
+      <c r="P22" s="13">
+        <f>N22^2</f>
+        <v>7396</v>
+      </c>
+    </row>
+    <row r="23" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N23" s="5">
+        <v>86.133333333333326</v>
+      </c>
+      <c r="P23" s="13">
+        <f>N23^2</f>
+        <v>7418.9511111111096</v>
+      </c>
+    </row>
+    <row r="24" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N24" s="5">
+        <v>86.333333333333329</v>
+      </c>
+      <c r="P24" s="13">
+        <f>N24^2</f>
+        <v>7453.4444444444434</v>
+      </c>
+    </row>
+    <row r="25" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N25" s="6">
+        <v>86.333333333333329</v>
+      </c>
+      <c r="P25" s="13">
+        <f>N25^2</f>
+        <v>7453.4444444444434</v>
+      </c>
+    </row>
+    <row r="26" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N26" s="5">
+        <v>86.666666666666671</v>
+      </c>
+      <c r="P26" s="13">
+        <f>N26^2</f>
+        <v>7511.1111111111122</v>
+      </c>
+    </row>
+    <row r="27" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N27" s="6">
+        <v>87</v>
+      </c>
+      <c r="P27" s="13">
+        <f>N27^2</f>
+        <v>7569</v>
+      </c>
+    </row>
+    <row r="28" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N28" s="6">
+        <v>88.666666666666671</v>
+      </c>
+      <c r="P28" s="13">
+        <f>N28^2</f>
+        <v>7861.7777777777783</v>
+      </c>
+    </row>
+    <row r="29" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N29" s="5">
+        <v>89.266666666666666</v>
+      </c>
+      <c r="P29" s="13">
+        <f>N29^2</f>
+        <v>7968.5377777777776</v>
+      </c>
+    </row>
+    <row r="30" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N30" s="5">
+        <v>89.466666666666654</v>
+      </c>
+      <c r="P30" s="13">
+        <f>N30^2</f>
+        <v>8004.2844444444427</v>
+      </c>
+    </row>
+    <row r="31" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N31" s="5">
+        <v>89.8</v>
+      </c>
+      <c r="P31" s="13">
+        <f>N31^2</f>
+        <v>8064.0399999999991</v>
+      </c>
+    </row>
+    <row r="32" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N32" s="5">
+        <v>89.933333333333337</v>
+      </c>
+      <c r="P32" s="13">
+        <f>N32^2</f>
+        <v>8088.0044444444447</v>
+      </c>
+    </row>
+    <row r="33" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N33" s="5">
+        <v>90.666666666666671</v>
+      </c>
+      <c r="P33" s="13">
+        <f>N33^2</f>
+        <v>8220.4444444444453</v>
+      </c>
+    </row>
+    <row r="34" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N34" s="5">
+        <v>90.8</v>
+      </c>
+      <c r="P34" s="13">
+        <f>N34^2</f>
+        <v>8244.64</v>
+      </c>
+    </row>
+    <row r="35" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N35" s="5">
+        <v>90.866666666666674</v>
+      </c>
+      <c r="P35" s="13">
+        <f>N35^2</f>
+        <v>8256.7511111111126</v>
+      </c>
+    </row>
+    <row r="36" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N36" s="5">
+        <v>91.066666666666663</v>
+      </c>
+      <c r="P36" s="13">
+        <f>N36^2</f>
+        <v>8293.137777777778</v>
+      </c>
+    </row>
+    <row r="37" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N37" s="5">
+        <v>91.533333333333346</v>
+      </c>
+      <c r="P37" s="13">
+        <f>N37^2</f>
+        <v>8378.3511111111129</v>
+      </c>
+    </row>
+    <row r="38" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N38" s="5">
+        <v>91.533333333333346</v>
+      </c>
+      <c r="P38" s="13">
+        <f>N38^2</f>
+        <v>8378.3511111111129</v>
+      </c>
+    </row>
+    <row r="39" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N39" s="5">
+        <v>92</v>
+      </c>
+      <c r="P39" s="13">
+        <f>N39^2</f>
+        <v>8464</v>
+      </c>
+    </row>
+    <row r="40" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N40" s="5">
+        <v>92.333333333333329</v>
+      </c>
+      <c r="P40" s="13">
+        <f>N40^2</f>
+        <v>8525.4444444444434</v>
+      </c>
+    </row>
+    <row r="41" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N41" s="5">
+        <v>92.733333333333334</v>
+      </c>
+      <c r="P41" s="13">
+        <f>N41^2</f>
+        <v>8599.4711111111119</v>
+      </c>
+    </row>
+    <row r="42" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N42" s="5">
+        <v>92.933333333333337</v>
+      </c>
+      <c r="P42" s="13">
+        <f>N42^2</f>
+        <v>8636.6044444444451</v>
+      </c>
+    </row>
+    <row r="43" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N43" s="5">
+        <v>93.2</v>
+      </c>
+      <c r="P43" s="13">
+        <f>N43^2</f>
+        <v>8686.24</v>
+      </c>
+    </row>
+    <row r="44" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N44" s="5">
+        <v>94</v>
+      </c>
+      <c r="P44" s="13">
+        <f>N44^2</f>
+        <v>8836</v>
+      </c>
+    </row>
+    <row r="45" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N45" s="5">
+        <v>94.066666666666663</v>
+      </c>
+      <c r="P45" s="13">
+        <f>N45^2</f>
+        <v>8848.5377777777776</v>
+      </c>
+    </row>
+    <row r="46" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N46" s="5">
+        <v>94.133333333333326</v>
+      </c>
+      <c r="P46" s="13">
+        <f>N46^2</f>
+        <v>8861.0844444444429</v>
+      </c>
+    </row>
+    <row r="47" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N47" s="5">
+        <v>94.600000000000009</v>
+      </c>
+      <c r="P47" s="13">
+        <f>N47^2</f>
+        <v>8949.1600000000017</v>
+      </c>
+    </row>
+    <row r="48" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N48" s="5">
+        <v>94.866666666666674</v>
+      </c>
+      <c r="P48" s="13">
+        <f>N48^2</f>
+        <v>8999.684444444445</v>
+      </c>
+    </row>
+    <row r="49" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N49" s="5">
+        <v>95.066666666666663</v>
+      </c>
+      <c r="P49" s="13">
+        <f>N49^2</f>
+        <v>9037.6711111111108</v>
+      </c>
+    </row>
+    <row r="50" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N50" s="6">
+        <v>95.666666666666671</v>
+      </c>
+      <c r="P50" s="13">
+        <f>N50^2</f>
+        <v>9152.1111111111113</v>
+      </c>
+    </row>
+    <row r="51" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N51" s="6">
+        <v>95.666666666666671</v>
+      </c>
+      <c r="P51" s="13">
+        <f>N51^2</f>
+        <v>9152.1111111111113</v>
+      </c>
+    </row>
+    <row r="52" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N52" s="5">
+        <v>96.466666666666654</v>
+      </c>
+      <c r="P52" s="13">
+        <f>N52^2</f>
+        <v>9305.8177777777746</v>
+      </c>
+    </row>
+    <row r="53" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N53" s="5">
+        <v>97.066666666666663</v>
+      </c>
+      <c r="P53" s="13">
+        <f>N53^2</f>
+        <v>9421.9377777777772</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4036,14 +5150,16 @@
   <dimension ref="B4:I15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="B4:F12"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="8" width="9.140625" style="2"/>
     <col min="9" max="9" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="2"/>
+    <col min="10" max="15" width="9.140625" style="2"/>
+    <col min="16" max="16" width="11.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
@@ -4238,13 +5354,7 @@
       </c>
     </row>
     <row r="15" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="H15" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="I15" s="2">
-        <f>SQRT(548.0075)</f>
-        <v>23.409560012951975</v>
-      </c>
+      <c r="H15" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4254,10 +5364,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="B1:J11"/>
+  <dimension ref="B1:O64"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4267,19 +5377,34 @@
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="25.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:15" x14ac:dyDescent="0.25">
       <c r="F1" s="23"/>
       <c r="G1" s="23"/>
       <c r="H1" s="23"/>
-    </row>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="L1" t="s">
+        <v>95</v>
+      </c>
+      <c r="M1">
+        <f>2/4*(50+1)</f>
+        <v>25.5</v>
+      </c>
+      <c r="N1" t="s">
+        <v>97</v>
+      </c>
+      <c r="O1" s="45">
+        <f>89</f>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="2:15" x14ac:dyDescent="0.25">
       <c r="F2" s="23"/>
       <c r="G2" s="23"/>
       <c r="H2" s="23"/>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B3" s="15" t="s">
         <v>34</v>
       </c>
@@ -4306,8 +5431,21 @@
       <c r="J3" s="27" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="L3" t="s">
+        <v>91</v>
+      </c>
+      <c r="M3">
+        <f>1/4*(50+1)</f>
+        <v>12.75</v>
+      </c>
+      <c r="N3" t="s">
+        <v>94</v>
+      </c>
+      <c r="O3" s="45">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B4" s="15" t="s">
         <v>36</v>
       </c>
@@ -4335,8 +5473,21 @@
       <c r="J4" s="26" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="L4" t="s">
+        <v>92</v>
+      </c>
+      <c r="M4">
+        <f>3/4*(50+1)</f>
+        <v>38.25</v>
+      </c>
+      <c r="N4" t="s">
+        <v>93</v>
+      </c>
+      <c r="O4" s="45">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B5" s="15" t="s">
         <v>37</v>
       </c>
@@ -4358,7 +5509,7 @@
       <c r="I5" s="26"/>
       <c r="J5" s="26"/>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B6" s="15" t="s">
         <v>38</v>
       </c>
@@ -4380,12 +5531,15 @@
         <v>53</v>
       </c>
       <c r="I6" s="28">
-        <f>D8+(((1/4*C11)-SUM(C4:C7))*F8)/C8</f>
+        <f>D8+(((1/4*C11)-SUM(C4:C7))/C8)*F8</f>
         <v>81.318181818181813</v>
       </c>
       <c r="J6" s="29"/>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B7" s="15" t="s">
         <v>39</v>
       </c>
@@ -4407,12 +5561,26 @@
         <v>54</v>
       </c>
       <c r="I7" s="30">
-        <f>D10+(((3/4*C11)-SUM(C4:C9))*F10)/C10</f>
+        <f>D10+(((3/4*C11)-SUM(C4:C9))/C10)*F10</f>
         <v>92.730769230769226</v>
       </c>
       <c r="J7" s="26"/>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K7">
+        <f>_xlfn.QUARTILE.EXC($C$15:$C$64,1)</f>
+        <v>82.816666666666663</v>
+      </c>
+      <c r="L7" t="s">
+        <v>91</v>
+      </c>
+      <c r="M7" t="s">
+        <v>99</v>
+      </c>
+      <c r="O7">
+        <f>(K9-K7)/2</f>
+        <v>4.9833333333333343</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B8" s="15" t="s">
         <v>40</v>
       </c>
@@ -4433,8 +5601,18 @@
       <c r="H8" s="26"/>
       <c r="I8" s="28"/>
       <c r="J8" s="26"/>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K8" s="2">
+        <f>_xlfn.QUARTILE.EXC($C$15:$C$64,2)</f>
+        <v>88.966666666666669</v>
+      </c>
+      <c r="L8" t="s">
+        <v>96</v>
+      </c>
+      <c r="M8" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B9" s="15" t="s">
         <v>41</v>
       </c>
@@ -4453,15 +5631,25 @@
         <v>6</v>
       </c>
       <c r="H9" s="26" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="I9" s="28">
         <f>1/2*(I7-I6)</f>
         <v>5.7062937062937067</v>
       </c>
       <c r="J9" s="26"/>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K9" s="2">
+        <f>_xlfn.QUARTILE.EXC($C$15:$C$64,3)</f>
+        <v>92.783333333333331</v>
+      </c>
+      <c r="L9" t="s">
+        <v>92</v>
+      </c>
+      <c r="M9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B10" s="15" t="s">
         <v>42</v>
       </c>
@@ -4480,7 +5668,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B11" s="21" t="s">
         <v>14</v>
       </c>
@@ -4490,6 +5678,270 @@
       </c>
       <c r="D11" s="20"/>
       <c r="E11" s="20"/>
+    </row>
+    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="H12" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C15" s="6">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C16" s="5">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C17" s="5">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C18" s="5">
+        <v>63.066666666666663</v>
+      </c>
+    </row>
+    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C19" s="6">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="20" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C20" s="6">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="21" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C21" s="6">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C22" s="6">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="23" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C23" s="5">
+        <v>79.466666666666669</v>
+      </c>
+    </row>
+    <row r="24" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C24" s="6">
+        <v>79.666666666666671</v>
+      </c>
+    </row>
+    <row r="25" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C25" s="6">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="26" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C26" s="6">
+        <v>80.666666666666671</v>
+      </c>
+    </row>
+    <row r="27" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C27" s="44">
+        <v>83.533333333333331</v>
+      </c>
+      <c r="D27" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="28" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C28" s="5">
+        <v>84.399999999999991</v>
+      </c>
+    </row>
+    <row r="29" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C29" s="5">
+        <v>84.600000000000009</v>
+      </c>
+    </row>
+    <row r="30" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C30" s="5">
+        <v>84.600000000000009</v>
+      </c>
+    </row>
+    <row r="31" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C31" s="6">
+        <v>85.666666666666671</v>
+      </c>
+    </row>
+    <row r="32" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C32" s="5">
+        <v>85.733333333333334</v>
+      </c>
+    </row>
+    <row r="33" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C33" s="5">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="34" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C34" s="5">
+        <v>86.133333333333326</v>
+      </c>
+    </row>
+    <row r="35" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C35" s="5">
+        <v>86.333333333333329</v>
+      </c>
+    </row>
+    <row r="36" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C36" s="6">
+        <v>86.333333333333329</v>
+      </c>
+    </row>
+    <row r="37" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C37" s="5">
+        <v>86.666666666666671</v>
+      </c>
+    </row>
+    <row r="38" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C38" s="6">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="39" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C39" s="46">
+        <v>88.666666666666671</v>
+      </c>
+      <c r="D39" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="40" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C40" s="5">
+        <v>89.266666666666666</v>
+      </c>
+    </row>
+    <row r="41" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C41" s="5">
+        <v>89.466666666666654</v>
+      </c>
+    </row>
+    <row r="42" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C42" s="5">
+        <v>89.8</v>
+      </c>
+    </row>
+    <row r="43" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C43" s="5">
+        <v>89.933333333333337</v>
+      </c>
+    </row>
+    <row r="44" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C44" s="5">
+        <v>90.666666666666671</v>
+      </c>
+    </row>
+    <row r="45" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C45" s="5">
+        <v>90.8</v>
+      </c>
+    </row>
+    <row r="46" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C46" s="5">
+        <v>90.866666666666674</v>
+      </c>
+    </row>
+    <row r="47" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C47" s="5">
+        <v>91.066666666666663</v>
+      </c>
+    </row>
+    <row r="48" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C48" s="5">
+        <v>91.533333333333346</v>
+      </c>
+    </row>
+    <row r="49" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C49" s="5">
+        <v>91.533333333333346</v>
+      </c>
+    </row>
+    <row r="50" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C50" s="5">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="51" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C51" s="5">
+        <v>92.333333333333329</v>
+      </c>
+    </row>
+    <row r="52" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C52" s="44">
+        <v>92.733333333333334</v>
+      </c>
+      <c r="D52" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="53" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C53" s="5">
+        <v>92.933333333333337</v>
+      </c>
+    </row>
+    <row r="54" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C54" s="5">
+        <v>93.2</v>
+      </c>
+    </row>
+    <row r="55" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C55" s="5">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="56" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C56" s="5">
+        <v>94.066666666666663</v>
+      </c>
+    </row>
+    <row r="57" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C57" s="5">
+        <v>94.133333333333326</v>
+      </c>
+    </row>
+    <row r="58" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C58" s="5">
+        <v>94.600000000000009</v>
+      </c>
+    </row>
+    <row r="59" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C59" s="5">
+        <v>94.866666666666674</v>
+      </c>
+    </row>
+    <row r="60" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C60" s="5">
+        <v>95.066666666666663</v>
+      </c>
+    </row>
+    <row r="61" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C61" s="6">
+        <v>95.666666666666671</v>
+      </c>
+    </row>
+    <row r="62" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C62" s="6">
+        <v>95.666666666666671</v>
+      </c>
+    </row>
+    <row r="63" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C63" s="5">
+        <v>96.466666666666654</v>
+      </c>
+    </row>
+    <row r="64" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C64" s="5">
+        <v>97.066666666666663</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4501,7 +5953,7 @@
   <dimension ref="B3:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
pembuatan versi makalah baru, penambahan data di excel
</commit_message>
<xml_diff>
--- a/Data Penyebaran Data Frekuensi Tugas Kelompok.xlsx
+++ b/Data Penyebaran Data Frekuensi Tugas Kelompok.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hamdi\Documents\statistikafiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FA89E4B-CCAD-4344-8747-27F917D6A8D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA539A3F-742C-4B24-9F84-9A65E962DB1F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="103">
   <si>
     <t>No. Urut</t>
   </si>
@@ -328,12 +328,6 @@
     <t>Tidak terpakai</t>
   </si>
   <si>
-    <t>Rata-rata</t>
-  </si>
-  <si>
-    <t>|xi​−xˉ|</t>
-  </si>
-  <si>
     <t>Hasil excel</t>
   </si>
   <si>
@@ -389,6 +383,15 @@
   </si>
   <si>
     <t>Kuartil Atas</t>
+  </si>
+  <si>
+    <t>Standar deviasi adalah nilai statistik yang digunakan untuk menentukan bagaimana sebaran data dalam sampel, dan seberapa dekat titik data individu ke mean – atau rata-rata – nilai sampel.</t>
+  </si>
+  <si>
+    <t>Sebuah standar deviasi dari kumpulan data sama dengan nol menunjukkan bahwa semua nilai-nilai dalam himpunan tersebut adalah sama. Sebuah nilai deviasi yang lebih besar akan memberikan makna bahwa titik data individu jauh dari nilai rata-rata.</t>
+  </si>
+  <si>
+    <t>Varian merupakan ukuran variabilitas data, yang berarti semakin besar nilai varian berarti semakin tinggi fluktuasi data antara satu data dengan data yang lain</t>
   </si>
 </sst>
 </file>
@@ -498,7 +501,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -526,6 +529,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -628,7 +637,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -700,15 +709,6 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -730,6 +730,18 @@
     <xf numFmtId="1" fontId="8" fillId="5" borderId="4" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Comma [0] 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -1352,6 +1364,441 @@
                 <a:t>) ̅</a:t>
               </a:r>
               <a:endParaRPr lang="en-ID" sz="1600"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="448007" cy="172227"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="5" name="TextBox 4">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3BF12990-DC9C-48E2-BF4D-1E69141D0454}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="8391525" y="604837"/>
+              <a:ext cx="448007" cy="172227"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:d>
+                      <m:dPr>
+                        <m:begChr m:val="|"/>
+                        <m:endChr m:val="|"/>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-ID" sz="1100" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:dPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-ID" sz="1100" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑥</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-ID" sz="1100" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>−</m:t>
+                        </m:r>
+                        <m:acc>
+                          <m:accPr>
+                            <m:chr m:val="̅"/>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-ID" sz="1100" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:accPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="en-ID" sz="1100" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑥</m:t>
+                            </m:r>
+                          </m:e>
+                        </m:acc>
+                      </m:e>
+                    </m:d>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-ID" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="5" name="TextBox 4">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3BF12990-DC9C-48E2-BF4D-1E69141D0454}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="8391525" y="604837"/>
+              <a:ext cx="448007" cy="172227"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-ID" sz="1100" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>|𝑥−𝑥 ̅ |</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-ID" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>1000125</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="495300" cy="219163"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="7" name="TextBox 6">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{92FD4D25-0A70-48BE-B987-1B947CFA34A5}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="8829675" y="161925"/>
+              <a:ext cx="495300" cy="219163"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:acc>
+                      <m:accPr>
+                        <m:chr m:val="̅"/>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-ID" sz="1400" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:accPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-ID" sz="1400" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑥</m:t>
+                        </m:r>
+                      </m:e>
+                    </m:acc>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-ID" sz="1600"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="7" name="TextBox 6">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{92FD4D25-0A70-48BE-B987-1B947CFA34A5}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="8829675" y="161925"/>
+              <a:ext cx="495300" cy="219163"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="en-ID" sz="1400" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑥 ̅</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-ID" sz="1600"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>185737</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="156133" cy="172227"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="8" name="TextBox 7">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{623986CF-942B-4A08-96D1-1E48016C5F03}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="7429500" y="566737"/>
+              <a:ext cx="156133" cy="172227"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>𝑥𝑖</m:t>
+                    </m:r>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-ID" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="8" name="TextBox 7">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{623986CF-942B-4A08-96D1-1E48016C5F03}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="7429500" y="566737"/>
+              <a:ext cx="156133" cy="172227"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑥𝑖</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-ID" sz="1100"/>
             </a:p>
           </xdr:txBody>
         </xdr:sp>
@@ -2480,7 +2927,7 @@
   <dimension ref="A1:M53"/>
   <sheetViews>
     <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="G55" sqref="G55"/>
+      <selection activeCell="I38" sqref="I38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2493,7 +2940,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="44" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
@@ -2501,7 +2948,7 @@
       </c>
     </row>
     <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="34"/>
+      <c r="A2" s="45"/>
       <c r="B2" s="8" t="s">
         <v>2</v>
       </c>
@@ -2996,10 +3443,10 @@
       <c r="B36" s="5">
         <v>91.066666666666663</v>
       </c>
-      <c r="H36" s="38" t="s">
+      <c r="H36" s="35" t="s">
         <v>66</v>
       </c>
-      <c r="I36" s="38"/>
+      <c r="I36" s="35"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
@@ -3008,8 +3455,8 @@
       <c r="B37" s="5">
         <v>91.533333333333346</v>
       </c>
-      <c r="H37" s="36"/>
-      <c r="I37" s="36"/>
+      <c r="H37" s="33"/>
+      <c r="I37" s="33"/>
     </row>
     <row r="38" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
@@ -3018,10 +3465,10 @@
       <c r="B38" s="5">
         <v>91.533333333333346</v>
       </c>
-      <c r="H38" s="36" t="s">
+      <c r="H38" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="I38" s="36">
+      <c r="I38" s="33">
         <v>85.705333333333328</v>
       </c>
     </row>
@@ -3032,10 +3479,10 @@
       <c r="B39" s="5">
         <v>92</v>
       </c>
-      <c r="H39" s="36" t="s">
+      <c r="H39" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="I39" s="36">
+      <c r="I39" s="33">
         <v>1.4179120928138926</v>
       </c>
     </row>
@@ -3046,10 +3493,10 @@
       <c r="B40" s="5">
         <v>92.333333333333329</v>
       </c>
-      <c r="H40" s="36" t="s">
+      <c r="H40" s="33" t="s">
         <v>69</v>
       </c>
-      <c r="I40" s="36">
+      <c r="I40" s="33">
         <v>88.966666666666669</v>
       </c>
     </row>
@@ -3060,10 +3507,10 @@
       <c r="B41" s="5">
         <v>92.733333333333334</v>
       </c>
-      <c r="H41" s="36" t="s">
+      <c r="H41" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="I41" s="36">
+      <c r="I41" s="33">
         <v>84.600000000000009</v>
       </c>
     </row>
@@ -3074,10 +3521,10 @@
       <c r="B42" s="5">
         <v>92.933333333333337</v>
       </c>
-      <c r="H42" s="36" t="s">
+      <c r="H42" s="33" t="s">
         <v>71</v>
       </c>
-      <c r="I42" s="36">
+      <c r="I42" s="33">
         <v>10.026152559551129</v>
       </c>
     </row>
@@ -3088,10 +3535,10 @@
       <c r="B43" s="5">
         <v>93.2</v>
       </c>
-      <c r="H43" s="36" t="s">
+      <c r="H43" s="33" t="s">
         <v>72</v>
       </c>
-      <c r="I43" s="36">
+      <c r="I43" s="33">
         <v>100.52373514739364</v>
       </c>
     </row>
@@ -3102,10 +3549,10 @@
       <c r="B44" s="5">
         <v>94</v>
       </c>
-      <c r="H44" s="36" t="s">
+      <c r="H44" s="33" t="s">
         <v>73</v>
       </c>
-      <c r="I44" s="36">
+      <c r="I44" s="33">
         <v>1.4547799557831986</v>
       </c>
     </row>
@@ -3116,10 +3563,10 @@
       <c r="B45" s="5">
         <v>94.066666666666663</v>
       </c>
-      <c r="H45" s="36" t="s">
+      <c r="H45" s="33" t="s">
         <v>74</v>
       </c>
-      <c r="I45" s="36">
+      <c r="I45" s="33">
         <v>-1.44069540750446</v>
       </c>
     </row>
@@ -3130,10 +3577,10 @@
       <c r="B46" s="5">
         <v>94.133333333333326</v>
       </c>
-      <c r="H46" s="36" t="s">
+      <c r="H46" s="33" t="s">
         <v>75</v>
       </c>
-      <c r="I46" s="36">
+      <c r="I46" s="33">
         <v>40.066666666666663</v>
       </c>
     </row>
@@ -3144,10 +3591,10 @@
       <c r="B47" s="5">
         <v>94.600000000000009</v>
       </c>
-      <c r="H47" s="36" t="s">
+      <c r="H47" s="33" t="s">
         <v>76</v>
       </c>
-      <c r="I47" s="36">
+      <c r="I47" s="33">
         <v>57</v>
       </c>
     </row>
@@ -3158,10 +3605,10 @@
       <c r="B48" s="5">
         <v>94.866666666666674</v>
       </c>
-      <c r="H48" s="36" t="s">
+      <c r="H48" s="33" t="s">
         <v>77</v>
       </c>
-      <c r="I48" s="36">
+      <c r="I48" s="33">
         <v>97.066666666666663</v>
       </c>
     </row>
@@ -3172,10 +3619,10 @@
       <c r="B49" s="5">
         <v>95.066666666666663</v>
       </c>
-      <c r="H49" s="36" t="s">
+      <c r="H49" s="33" t="s">
         <v>78</v>
       </c>
-      <c r="I49" s="36">
+      <c r="I49" s="33">
         <v>4285.2666666666664</v>
       </c>
     </row>
@@ -3186,10 +3633,10 @@
       <c r="B50" s="6">
         <v>95.666666666666671</v>
       </c>
-      <c r="H50" s="37" t="s">
+      <c r="H50" s="34" t="s">
         <v>79</v>
       </c>
-      <c r="I50" s="37">
+      <c r="I50" s="34">
         <v>50</v>
       </c>
     </row>
@@ -3237,7 +3684,7 @@
   <dimension ref="B1:S17"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="R3" sqref="R3"/>
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3250,15 +3697,15 @@
       <c r="B1" t="s">
         <v>28</v>
       </c>
-      <c r="M1" s="39" t="s">
+      <c r="M1" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="N1" s="39"/>
-      <c r="O1" s="39"/>
-      <c r="P1" s="39"/>
-      <c r="Q1" s="39"/>
-      <c r="R1" s="39"/>
-      <c r="S1" s="39"/>
+      <c r="N1" s="36"/>
+      <c r="O1" s="36"/>
+      <c r="P1" s="36"/>
+      <c r="Q1" s="36"/>
+      <c r="R1" s="36"/>
+      <c r="S1" s="36"/>
     </row>
     <row r="2" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B2" s="5">
@@ -3291,15 +3738,15 @@
       <c r="K2" s="5">
         <v>93.2</v>
       </c>
-      <c r="M2" s="39" t="s">
+      <c r="M2" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="N2" s="39"/>
-      <c r="O2" s="39"/>
-      <c r="P2" s="39"/>
-      <c r="Q2" s="39"/>
-      <c r="R2" s="39"/>
-      <c r="S2" s="39"/>
+      <c r="N2" s="36"/>
+      <c r="O2" s="36"/>
+      <c r="P2" s="36"/>
+      <c r="Q2" s="36"/>
+      <c r="R2" s="36"/>
+      <c r="S2" s="36"/>
     </row>
     <row r="3" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B3" s="5">
@@ -3332,21 +3779,21 @@
       <c r="K3" s="5">
         <v>90.666666666666671</v>
       </c>
-      <c r="M3" s="39" t="s">
+      <c r="M3" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="N3" s="39"/>
-      <c r="O3" s="39"/>
-      <c r="P3" s="39"/>
-      <c r="Q3" s="39">
+      <c r="N3" s="36"/>
+      <c r="O3" s="36"/>
+      <c r="P3" s="36"/>
+      <c r="Q3" s="36">
         <f xml:space="preserve"> 1+ 3.3 * LOG(50)</f>
         <v>6.6066010143088612</v>
       </c>
-      <c r="R3" s="40">
+      <c r="R3" s="37">
         <f>Q3</f>
         <v>6.6066010143088612</v>
       </c>
-      <c r="S3" s="39"/>
+      <c r="S3" s="36"/>
     </row>
     <row r="4" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B4" s="6">
@@ -3379,18 +3826,18 @@
       <c r="K4" s="5">
         <v>86.133333333333326</v>
       </c>
-      <c r="M4" s="39" t="s">
+      <c r="M4" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="N4" s="39"/>
-      <c r="O4" s="39"/>
-      <c r="P4" s="39"/>
-      <c r="Q4" s="40">
+      <c r="N4" s="36"/>
+      <c r="O4" s="36"/>
+      <c r="P4" s="36"/>
+      <c r="Q4" s="37">
         <f>K14-B10</f>
         <v>40.066666666666663</v>
       </c>
-      <c r="R4" s="39"/>
-      <c r="S4" s="39"/>
+      <c r="R4" s="36"/>
+      <c r="S4" s="36"/>
     </row>
     <row r="5" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B5" s="5">
@@ -3423,21 +3870,21 @@
       <c r="K5" s="5">
         <v>97.066666666666663</v>
       </c>
-      <c r="M5" s="39" t="s">
+      <c r="M5" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="N5" s="39"/>
-      <c r="O5" s="39"/>
-      <c r="P5" s="39"/>
-      <c r="Q5" s="39">
+      <c r="N5" s="36"/>
+      <c r="O5" s="36"/>
+      <c r="P5" s="36"/>
+      <c r="Q5" s="36">
         <f>Q4/R3</f>
         <v>6.0646414971766189</v>
       </c>
-      <c r="R5" s="40">
+      <c r="R5" s="37">
         <f>Q5</f>
         <v>6.0646414971766189</v>
       </c>
-      <c r="S5" s="39"/>
+      <c r="S5" s="36"/>
     </row>
     <row r="6" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B6" s="6">
@@ -3470,55 +3917,55 @@
       <c r="K6" s="6">
         <v>79.666666666666671</v>
       </c>
-      <c r="M6" s="39"/>
-      <c r="N6" s="39"/>
-      <c r="O6" s="39"/>
-      <c r="P6" s="39"/>
-      <c r="Q6" s="39"/>
-      <c r="R6" s="39"/>
-      <c r="S6" s="39"/>
+      <c r="M6" s="36"/>
+      <c r="N6" s="36"/>
+      <c r="O6" s="36"/>
+      <c r="P6" s="36"/>
+      <c r="Q6" s="36"/>
+      <c r="R6" s="36"/>
+      <c r="S6" s="36"/>
     </row>
     <row r="7" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="M7" s="41" t="s">
+      <c r="M7" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="N7" s="41" t="s">
+      <c r="N7" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="O7" s="39"/>
-      <c r="P7" s="39"/>
-      <c r="Q7" s="39"/>
-      <c r="R7" s="39"/>
-      <c r="S7" s="39"/>
+      <c r="O7" s="36"/>
+      <c r="P7" s="36"/>
+      <c r="Q7" s="36"/>
+      <c r="R7" s="36"/>
+      <c r="S7" s="36"/>
     </row>
     <row r="8" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="M8" s="41" t="s">
+      <c r="M8" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="N8" s="41">
+      <c r="N8" s="38">
         <v>3</v>
       </c>
-      <c r="O8" s="39"/>
-      <c r="P8" s="39"/>
-      <c r="Q8" s="39"/>
-      <c r="R8" s="39"/>
-      <c r="S8" s="39"/>
+      <c r="O8" s="36"/>
+      <c r="P8" s="36"/>
+      <c r="Q8" s="36"/>
+      <c r="R8" s="36"/>
+      <c r="S8" s="36"/>
     </row>
     <row r="9" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>27</v>
       </c>
-      <c r="M9" s="41" t="s">
+      <c r="M9" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="N9" s="41">
+      <c r="N9" s="38">
         <v>2</v>
       </c>
-      <c r="O9" s="39"/>
-      <c r="P9" s="39"/>
-      <c r="Q9" s="39"/>
-      <c r="R9" s="39"/>
-      <c r="S9" s="39"/>
+      <c r="O9" s="36"/>
+      <c r="P9" s="36"/>
+      <c r="Q9" s="36"/>
+      <c r="R9" s="36"/>
+      <c r="S9" s="36"/>
     </row>
     <row r="10" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B10" s="6">
@@ -3551,17 +3998,17 @@
       <c r="K10" s="6">
         <v>79.666666666666671</v>
       </c>
-      <c r="M10" s="41" t="s">
+      <c r="M10" s="38" t="s">
         <v>38</v>
       </c>
-      <c r="N10" s="41">
+      <c r="N10" s="38">
         <v>2</v>
       </c>
-      <c r="O10" s="39"/>
-      <c r="P10" s="39"/>
-      <c r="Q10" s="39"/>
-      <c r="R10" s="39"/>
-      <c r="S10" s="39"/>
+      <c r="O10" s="36"/>
+      <c r="P10" s="36"/>
+      <c r="Q10" s="36"/>
+      <c r="R10" s="36"/>
+      <c r="S10" s="36"/>
     </row>
     <row r="11" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B11" s="6">
@@ -3594,17 +4041,17 @@
       <c r="K11" s="5">
         <v>86.133333333333326</v>
       </c>
-      <c r="M11" s="41" t="s">
+      <c r="M11" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="N11" s="42">
+      <c r="N11" s="39">
         <v>4</v>
       </c>
-      <c r="O11" s="39"/>
-      <c r="P11" s="39"/>
-      <c r="Q11" s="39"/>
-      <c r="R11" s="39"/>
-      <c r="S11" s="39"/>
+      <c r="O11" s="36"/>
+      <c r="P11" s="36"/>
+      <c r="Q11" s="36"/>
+      <c r="R11" s="36"/>
+      <c r="S11" s="36"/>
     </row>
     <row r="12" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B12" s="5">
@@ -3637,17 +4084,17 @@
       <c r="K12" s="5">
         <v>90.666666666666671</v>
       </c>
-      <c r="M12" s="41" t="s">
+      <c r="M12" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="N12" s="41">
+      <c r="N12" s="38">
         <v>11</v>
       </c>
-      <c r="O12" s="39"/>
-      <c r="P12" s="39"/>
-      <c r="Q12" s="39"/>
-      <c r="R12" s="39"/>
-      <c r="S12" s="39"/>
+      <c r="O12" s="36"/>
+      <c r="P12" s="36"/>
+      <c r="Q12" s="36"/>
+      <c r="R12" s="36"/>
+      <c r="S12" s="36"/>
     </row>
     <row r="13" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B13" s="5">
@@ -3680,17 +4127,17 @@
       <c r="K13" s="5">
         <v>93.2</v>
       </c>
-      <c r="M13" s="41" t="s">
+      <c r="M13" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="N13" s="41">
+      <c r="N13" s="38">
         <v>15</v>
       </c>
-      <c r="O13" s="39"/>
-      <c r="P13" s="39"/>
-      <c r="Q13" s="39"/>
-      <c r="R13" s="39"/>
-      <c r="S13" s="39"/>
+      <c r="O13" s="36"/>
+      <c r="P13" s="36"/>
+      <c r="Q13" s="36"/>
+      <c r="R13" s="36"/>
+      <c r="S13" s="36"/>
     </row>
     <row r="14" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B14" s="5">
@@ -3723,34 +4170,34 @@
       <c r="K14" s="5">
         <v>97.066666666666663</v>
       </c>
-      <c r="M14" s="41" t="s">
+      <c r="M14" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="N14" s="41">
+      <c r="N14" s="38">
         <v>13</v>
       </c>
-      <c r="O14" s="39"/>
-      <c r="P14" s="39"/>
-      <c r="Q14" s="39"/>
-      <c r="R14" s="39"/>
-      <c r="S14" s="39"/>
+      <c r="O14" s="36"/>
+      <c r="P14" s="36"/>
+      <c r="Q14" s="36"/>
+      <c r="R14" s="36"/>
+      <c r="S14" s="36"/>
     </row>
     <row r="15" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="M15" s="41" t="s">
+      <c r="M15" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="N15" s="41">
+      <c r="N15" s="38">
         <f>SUM(N8:N14)</f>
         <v>50</v>
       </c>
-      <c r="O15" s="39"/>
-      <c r="P15" s="39"/>
-      <c r="Q15" s="39"/>
-      <c r="R15" s="39"/>
-      <c r="S15" s="39"/>
+      <c r="O15" s="36"/>
+      <c r="P15" s="36"/>
+      <c r="Q15" s="36"/>
+      <c r="R15" s="36"/>
+      <c r="S15" s="36"/>
     </row>
     <row r="17" spans="14:15" x14ac:dyDescent="0.25">
-      <c r="N17" s="39"/>
+      <c r="N17" s="36"/>
       <c r="O17" t="s">
         <v>80</v>
       </c>
@@ -3762,10 +4209,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A2:R54"/>
+  <dimension ref="A2:R55"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5:L54"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3773,26 +4220,26 @@
     <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.42578125" customWidth="1"/>
     <col min="7" max="7" width="14.28515625" customWidth="1"/>
-    <col min="13" max="13" width="21.140625" style="43" customWidth="1"/>
-    <col min="16" max="16" width="9.140625" style="43"/>
+    <col min="13" max="13" width="21.140625" style="40" customWidth="1"/>
+    <col min="16" max="16" width="9.140625" style="40"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="M2" s="43"/>
-      <c r="P2" s="43"/>
+      <c r="M2" s="40"/>
+      <c r="P2" s="40" t="s">
+        <v>45</v>
+      </c>
       <c r="R2" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="2:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="M3" s="43">
+      <c r="M3" s="40">
         <f>SUM(L5:L54)/50</f>
         <v>85.705333333333328</v>
       </c>
-      <c r="N3" t="s">
-        <v>81</v>
-      </c>
-      <c r="P3" s="43">
+      <c r="N3"/>
+      <c r="P3" s="40">
         <f>SUM(M5:M54)/50</f>
         <v>7.3729600000000017</v>
       </c>
@@ -3802,10 +4249,7 @@
       </c>
     </row>
     <row r="4" spans="2:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="M4" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="P4" s="43"/>
+      <c r="P4" s="40"/>
     </row>
     <row r="5" spans="2:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="15" t="s">
@@ -3825,7 +4269,7 @@
       <c r="L5" s="6">
         <v>57</v>
       </c>
-      <c r="M5" s="43">
+      <c r="M5" s="47">
         <f>ABS(L5-$M$3)</f>
         <v>28.705333333333328</v>
       </c>
@@ -3856,7 +4300,7 @@
       <c r="L6" s="5">
         <v>60</v>
       </c>
-      <c r="M6" s="43">
+      <c r="M6" s="47">
         <f t="shared" ref="M6:M54" si="0">ABS(L6-$M$3)</f>
         <v>25.705333333333328</v>
       </c>
@@ -3887,7 +4331,7 @@
       <c r="L7" s="5">
         <v>62</v>
       </c>
-      <c r="M7" s="43">
+      <c r="M7" s="47">
         <f t="shared" si="0"/>
         <v>23.705333333333328</v>
       </c>
@@ -3918,7 +4362,7 @@
       <c r="L8" s="5">
         <v>63.066666666666663</v>
       </c>
-      <c r="M8" s="43">
+      <c r="M8" s="47">
         <f t="shared" si="0"/>
         <v>22.638666666666666</v>
       </c>
@@ -3949,7 +4393,7 @@
       <c r="L9" s="6">
         <v>66</v>
       </c>
-      <c r="M9" s="43">
+      <c r="M9" s="47">
         <f t="shared" si="0"/>
         <v>19.705333333333328</v>
       </c>
@@ -3980,7 +4424,7 @@
       <c r="L10" s="6">
         <v>70</v>
       </c>
-      <c r="M10" s="43">
+      <c r="M10" s="47">
         <f t="shared" si="0"/>
         <v>15.705333333333328</v>
       </c>
@@ -4011,7 +4455,7 @@
       <c r="L11" s="6">
         <v>74</v>
       </c>
-      <c r="M11" s="43">
+      <c r="M11" s="47">
         <f t="shared" si="0"/>
         <v>11.705333333333328</v>
       </c>
@@ -4042,7 +4486,7 @@
       <c r="L12" s="6">
         <v>78</v>
       </c>
-      <c r="M12" s="43">
+      <c r="M12" s="47">
         <f t="shared" si="0"/>
         <v>7.7053333333333285</v>
       </c>
@@ -4068,7 +4512,7 @@
       <c r="L13" s="5">
         <v>79.466666666666669</v>
       </c>
-      <c r="M13" s="43">
+      <c r="M13" s="47">
         <f t="shared" si="0"/>
         <v>6.2386666666666599</v>
       </c>
@@ -4077,7 +4521,7 @@
       <c r="L14" s="6">
         <v>79.666666666666671</v>
       </c>
-      <c r="M14" s="43">
+      <c r="M14" s="47">
         <f t="shared" si="0"/>
         <v>6.0386666666666571</v>
       </c>
@@ -4086,7 +4530,7 @@
       <c r="L15" s="6">
         <v>80</v>
       </c>
-      <c r="M15" s="43">
+      <c r="M15" s="47">
         <f t="shared" si="0"/>
         <v>5.7053333333333285</v>
       </c>
@@ -4099,16 +4543,16 @@
       <c r="L16" s="6">
         <v>80.666666666666671</v>
       </c>
-      <c r="M16" s="43">
+      <c r="M16" s="47">
         <f t="shared" si="0"/>
         <v>5.0386666666666571</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="35" t="s">
+      <c r="A17" s="46" t="s">
         <v>46</v>
       </c>
-      <c r="B17" s="35"/>
+      <c r="B17" s="46"/>
       <c r="C17" s="17" t="s">
         <v>45</v>
       </c>
@@ -4119,31 +4563,31 @@
       <c r="L17" s="5">
         <v>83.533333333333331</v>
       </c>
-      <c r="M17" s="43">
+      <c r="M17" s="47">
         <f t="shared" si="0"/>
         <v>2.171999999999997</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E18" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="L18" s="5">
         <v>84.399999999999991</v>
       </c>
-      <c r="M18" s="43">
+      <c r="M18" s="47">
         <f t="shared" si="0"/>
         <v>1.305333333333337</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="L19" s="5">
         <v>84.600000000000009</v>
       </c>
-      <c r="M19" s="43">
+      <c r="M19" s="47">
         <f t="shared" si="0"/>
         <v>1.10533333333332</v>
       </c>
@@ -4152,7 +4596,7 @@
       <c r="L20" s="5">
         <v>84.600000000000009</v>
       </c>
-      <c r="M20" s="43">
+      <c r="M20" s="47">
         <f t="shared" si="0"/>
         <v>1.10533333333332</v>
       </c>
@@ -4161,7 +4605,7 @@
       <c r="L21" s="6">
         <v>85.666666666666671</v>
       </c>
-      <c r="M21" s="43">
+      <c r="M21" s="47">
         <f t="shared" si="0"/>
         <v>3.8666666666657079E-2</v>
       </c>
@@ -4170,7 +4614,7 @@
       <c r="L22" s="5">
         <v>85.733333333333334</v>
       </c>
-      <c r="M22" s="43">
+      <c r="M22" s="47">
         <f t="shared" si="0"/>
         <v>2.8000000000005798E-2</v>
       </c>
@@ -4179,7 +4623,7 @@
       <c r="L23" s="5">
         <v>86</v>
       </c>
-      <c r="M23" s="43">
+      <c r="M23" s="47">
         <f t="shared" si="0"/>
         <v>0.29466666666667152</v>
       </c>
@@ -4188,7 +4632,7 @@
       <c r="L24" s="5">
         <v>86.133333333333326</v>
       </c>
-      <c r="M24" s="43">
+      <c r="M24" s="47">
         <f t="shared" si="0"/>
         <v>0.42799999999999727</v>
       </c>
@@ -4197,7 +4641,7 @@
       <c r="L25" s="5">
         <v>86.333333333333329</v>
       </c>
-      <c r="M25" s="43">
+      <c r="M25" s="47">
         <f t="shared" si="0"/>
         <v>0.62800000000000011</v>
       </c>
@@ -4206,7 +4650,7 @@
       <c r="L26" s="6">
         <v>86.333333333333329</v>
       </c>
-      <c r="M26" s="43">
+      <c r="M26" s="47">
         <f t="shared" si="0"/>
         <v>0.62800000000000011</v>
       </c>
@@ -4215,7 +4659,7 @@
       <c r="L27" s="5">
         <v>86.666666666666671</v>
       </c>
-      <c r="M27" s="43">
+      <c r="M27" s="47">
         <f t="shared" si="0"/>
         <v>0.96133333333334292</v>
       </c>
@@ -4224,7 +4668,7 @@
       <c r="L28" s="6">
         <v>87</v>
       </c>
-      <c r="M28" s="43">
+      <c r="M28" s="47">
         <f t="shared" si="0"/>
         <v>1.2946666666666715</v>
       </c>
@@ -4233,7 +4677,7 @@
       <c r="L29" s="6">
         <v>88.666666666666671</v>
       </c>
-      <c r="M29" s="43">
+      <c r="M29" s="47">
         <f t="shared" si="0"/>
         <v>2.9613333333333429</v>
       </c>
@@ -4242,7 +4686,7 @@
       <c r="L30" s="5">
         <v>89.266666666666666</v>
       </c>
-      <c r="M30" s="43">
+      <c r="M30" s="47">
         <f t="shared" si="0"/>
         <v>3.5613333333333372</v>
       </c>
@@ -4251,7 +4695,7 @@
       <c r="L31" s="5">
         <v>89.466666666666654</v>
       </c>
-      <c r="M31" s="43">
+      <c r="M31" s="47">
         <f t="shared" si="0"/>
         <v>3.7613333333333259</v>
       </c>
@@ -4260,7 +4704,7 @@
       <c r="L32" s="5">
         <v>89.8</v>
       </c>
-      <c r="M32" s="43">
+      <c r="M32" s="47">
         <f t="shared" si="0"/>
         <v>4.0946666666666687</v>
       </c>
@@ -4269,7 +4713,7 @@
       <c r="L33" s="5">
         <v>89.933333333333337</v>
       </c>
-      <c r="M33" s="43">
+      <c r="M33" s="47">
         <f t="shared" si="0"/>
         <v>4.2280000000000086</v>
       </c>
@@ -4278,7 +4722,7 @@
       <c r="L34" s="5">
         <v>90.666666666666671</v>
       </c>
-      <c r="M34" s="43">
+      <c r="M34" s="47">
         <f t="shared" si="0"/>
         <v>4.9613333333333429</v>
       </c>
@@ -4287,7 +4731,7 @@
       <c r="L35" s="5">
         <v>90.8</v>
       </c>
-      <c r="M35" s="43">
+      <c r="M35" s="47">
         <f t="shared" si="0"/>
         <v>5.0946666666666687</v>
       </c>
@@ -4296,7 +4740,7 @@
       <c r="L36" s="5">
         <v>90.866666666666674</v>
       </c>
-      <c r="M36" s="43">
+      <c r="M36" s="47">
         <f t="shared" si="0"/>
         <v>5.1613333333333458</v>
       </c>
@@ -4305,7 +4749,7 @@
       <c r="L37" s="5">
         <v>91.066666666666663</v>
       </c>
-      <c r="M37" s="43">
+      <c r="M37" s="47">
         <f t="shared" si="0"/>
         <v>5.3613333333333344</v>
       </c>
@@ -4314,7 +4758,7 @@
       <c r="L38" s="5">
         <v>91.533333333333346</v>
       </c>
-      <c r="M38" s="43">
+      <c r="M38" s="47">
         <f t="shared" si="0"/>
         <v>5.8280000000000172</v>
       </c>
@@ -4323,7 +4767,7 @@
       <c r="L39" s="5">
         <v>91.533333333333346</v>
       </c>
-      <c r="M39" s="43">
+      <c r="M39" s="47">
         <f t="shared" si="0"/>
         <v>5.8280000000000172</v>
       </c>
@@ -4332,7 +4776,7 @@
       <c r="L40" s="5">
         <v>92</v>
       </c>
-      <c r="M40" s="43">
+      <c r="M40" s="47">
         <f t="shared" si="0"/>
         <v>6.2946666666666715</v>
       </c>
@@ -4341,7 +4785,7 @@
       <c r="L41" s="5">
         <v>92.333333333333329</v>
       </c>
-      <c r="M41" s="43">
+      <c r="M41" s="47">
         <f t="shared" si="0"/>
         <v>6.6280000000000001</v>
       </c>
@@ -4350,7 +4794,7 @@
       <c r="L42" s="5">
         <v>92.733333333333334</v>
       </c>
-      <c r="M42" s="43">
+      <c r="M42" s="47">
         <f t="shared" si="0"/>
         <v>7.0280000000000058</v>
       </c>
@@ -4359,7 +4803,7 @@
       <c r="L43" s="5">
         <v>92.933333333333337</v>
       </c>
-      <c r="M43" s="43">
+      <c r="M43" s="47">
         <f t="shared" si="0"/>
         <v>7.2280000000000086</v>
       </c>
@@ -4368,7 +4812,7 @@
       <c r="L44" s="5">
         <v>93.2</v>
       </c>
-      <c r="M44" s="43">
+      <c r="M44" s="47">
         <f t="shared" si="0"/>
         <v>7.4946666666666744</v>
       </c>
@@ -4377,7 +4821,7 @@
       <c r="L45" s="5">
         <v>94</v>
       </c>
-      <c r="M45" s="43">
+      <c r="M45" s="47">
         <f t="shared" si="0"/>
         <v>8.2946666666666715</v>
       </c>
@@ -4386,7 +4830,7 @@
       <c r="L46" s="5">
         <v>94.066666666666663</v>
       </c>
-      <c r="M46" s="43">
+      <c r="M46" s="47">
         <f t="shared" si="0"/>
         <v>8.3613333333333344</v>
       </c>
@@ -4395,7 +4839,7 @@
       <c r="L47" s="5">
         <v>94.133333333333326</v>
       </c>
-      <c r="M47" s="43">
+      <c r="M47" s="47">
         <f t="shared" si="0"/>
         <v>8.4279999999999973</v>
       </c>
@@ -4404,7 +4848,7 @@
       <c r="L48" s="5">
         <v>94.600000000000009</v>
       </c>
-      <c r="M48" s="43">
+      <c r="M48" s="47">
         <f t="shared" si="0"/>
         <v>8.89466666666668</v>
       </c>
@@ -4413,7 +4857,7 @@
       <c r="L49" s="5">
         <v>94.866666666666674</v>
       </c>
-      <c r="M49" s="43">
+      <c r="M49" s="47">
         <f t="shared" si="0"/>
         <v>9.1613333333333458</v>
       </c>
@@ -4422,7 +4866,7 @@
       <c r="L50" s="5">
         <v>95.066666666666663</v>
       </c>
-      <c r="M50" s="43">
+      <c r="M50" s="47">
         <f t="shared" si="0"/>
         <v>9.3613333333333344</v>
       </c>
@@ -4431,7 +4875,7 @@
       <c r="L51" s="6">
         <v>95.666666666666671</v>
       </c>
-      <c r="M51" s="43">
+      <c r="M51" s="47">
         <f t="shared" si="0"/>
         <v>9.9613333333333429</v>
       </c>
@@ -4440,7 +4884,7 @@
       <c r="L52" s="6">
         <v>95.666666666666671</v>
       </c>
-      <c r="M52" s="43">
+      <c r="M52" s="47">
         <f t="shared" si="0"/>
         <v>9.9613333333333429</v>
       </c>
@@ -4449,7 +4893,7 @@
       <c r="L53" s="5">
         <v>96.466666666666654</v>
       </c>
-      <c r="M53" s="43">
+      <c r="M53" s="47">
         <f t="shared" si="0"/>
         <v>10.761333333333326</v>
       </c>
@@ -4458,9 +4902,19 @@
       <c r="L54" s="5">
         <v>97.066666666666663</v>
       </c>
-      <c r="M54" s="43">
+      <c r="M54" s="47">
         <f t="shared" si="0"/>
         <v>11.361333333333334</v>
+      </c>
+    </row>
+    <row r="55" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L55" s="48">
+        <f>SUM(L5:L54)</f>
+        <v>4285.2666666666664</v>
+      </c>
+      <c r="M55" s="49">
+        <f>SUM(M5:M54)</f>
+        <v>368.64800000000008</v>
       </c>
     </row>
   </sheetData>
@@ -4475,31 +4929,33 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="B3:R53"/>
+  <dimension ref="A3:R53"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4:N53"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="8" width="9.140625" style="2"/>
     <col min="9" max="9" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="2"/>
+    <col min="10" max="16" width="9.140625" style="2"/>
+    <col min="17" max="17" width="14.85546875" style="2" customWidth="1"/>
+    <col min="18" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="O3" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B4" s="15" t="s">
         <v>34</v>
       </c>
@@ -4521,7 +4977,7 @@
         <v>4285.2666666666664</v>
       </c>
       <c r="P4" s="13">
-        <f>N4^2</f>
+        <f t="shared" ref="P4:P35" si="0">N4^2</f>
         <v>3249</v>
       </c>
       <c r="Q4" s="13">
@@ -4533,7 +4989,7 @@
         <v>18363510.404444441</v>
       </c>
     </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B5" s="15" t="s">
         <v>36</v>
       </c>
@@ -4556,11 +5012,11 @@
         <v>60</v>
       </c>
       <c r="P5" s="13">
-        <f>N5^2</f>
+        <f t="shared" si="0"/>
         <v>3600</v>
       </c>
     </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B6" s="15" t="s">
         <v>37</v>
       </c>
@@ -4572,22 +5028,26 @@
         <v>65.5</v>
       </c>
       <c r="E6" s="16">
-        <f t="shared" ref="E6:E11" si="0">C6*D6</f>
+        <f t="shared" ref="E6:E11" si="1">C6*D6</f>
         <v>131</v>
       </c>
       <c r="F6" s="16">
-        <f t="shared" ref="F6:F11" si="1">(ABS(D6-$D$16))</f>
+        <f t="shared" ref="F6:F11" si="2">(ABS(D6-$D$16))</f>
         <v>65.5</v>
+      </c>
+      <c r="L6" s="2">
+        <f>50*Q4</f>
+        <v>18609793.555555556</v>
       </c>
       <c r="N6" s="5">
         <v>62</v>
       </c>
       <c r="P6" s="13">
-        <f>N6^2</f>
+        <f t="shared" si="0"/>
         <v>3844</v>
       </c>
     </row>
-    <row r="7" spans="2:18" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B7" s="15" t="s">
         <v>38</v>
       </c>
@@ -4599,11 +5059,11 @@
         <v>71.5</v>
       </c>
       <c r="E7" s="16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>143</v>
       </c>
       <c r="F7" s="16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>71.5</v>
       </c>
       <c r="H7" s="19" t="s">
@@ -4613,15 +5073,19 @@
         <f>(C12*(F12^2))/(C12-1)</f>
         <v>300312.5</v>
       </c>
+      <c r="L7" s="13">
+        <f>L6-R4</f>
+        <v>246283.15111111477</v>
+      </c>
       <c r="N7" s="5">
         <v>63.066666666666663</v>
       </c>
       <c r="P7" s="13">
-        <f>N7^2</f>
+        <f t="shared" si="0"/>
         <v>3977.4044444444439</v>
       </c>
     </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B8" s="15" t="s">
         <v>39</v>
       </c>
@@ -4633,22 +5097,22 @@
         <v>77.5</v>
       </c>
       <c r="E8" s="16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>310</v>
       </c>
       <c r="F8" s="16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>77.5</v>
       </c>
       <c r="N8" s="6">
         <v>66</v>
       </c>
       <c r="P8" s="13">
-        <f>N8^2</f>
+        <f t="shared" si="0"/>
         <v>4356</v>
       </c>
     </row>
-    <row r="9" spans="2:18" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B9" s="15" t="s">
         <v>40</v>
       </c>
@@ -4660,15 +5124,15 @@
         <v>83.5</v>
       </c>
       <c r="E9" s="16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>918.5</v>
       </c>
       <c r="F9" s="16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>83.5</v>
       </c>
       <c r="H9" s="18" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="I9" s="2">
         <f>((50*Variansi!Q4)-Variansi!R4)/(50*49)</f>
@@ -4678,11 +5142,11 @@
         <v>70</v>
       </c>
       <c r="P9" s="13">
-        <f>N9^2</f>
+        <f t="shared" si="0"/>
         <v>4900</v>
       </c>
     </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B10" s="15" t="s">
         <v>41</v>
       </c>
@@ -4694,22 +5158,22 @@
         <v>89.5</v>
       </c>
       <c r="E10" s="16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1342.5</v>
       </c>
       <c r="F10" s="16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>89.5</v>
       </c>
       <c r="N10" s="6">
         <v>74</v>
       </c>
       <c r="P10" s="13">
-        <f>N10^2</f>
+        <f t="shared" si="0"/>
         <v>5476</v>
       </c>
     </row>
-    <row r="11" spans="2:18" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B11" s="15" t="s">
         <v>42</v>
       </c>
@@ -4721,15 +5185,15 @@
         <v>95.5</v>
       </c>
       <c r="E11" s="16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1241.5</v>
       </c>
       <c r="F11" s="16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>95.5</v>
       </c>
       <c r="H11" s="18" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="I11" s="2">
         <f>SQRT(I9)</f>
@@ -4739,11 +5203,11 @@
         <v>78</v>
       </c>
       <c r="P11" s="13">
-        <f>N11^2</f>
+        <f t="shared" si="0"/>
         <v>6084</v>
       </c>
     </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B12" s="15" t="s">
         <v>14</v>
       </c>
@@ -4764,44 +5228,47 @@
         <v>79.466666666666669</v>
       </c>
       <c r="P12" s="13">
-        <f>N12^2</f>
+        <f t="shared" si="0"/>
         <v>6314.9511111111115</v>
       </c>
     </row>
-    <row r="13" spans="2:18" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
       <c r="H13" s="18"/>
       <c r="N13" s="6">
         <v>79.666666666666671</v>
       </c>
       <c r="P13" s="13">
-        <f>N13^2</f>
+        <f t="shared" si="0"/>
         <v>6346.7777777777783</v>
       </c>
     </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="N14" s="6">
         <v>80</v>
       </c>
       <c r="P14" s="13">
-        <f>N14^2</f>
+        <f t="shared" si="0"/>
         <v>6400</v>
       </c>
     </row>
-    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>102</v>
+      </c>
       <c r="N15" s="6">
         <v>80.666666666666671</v>
       </c>
       <c r="P15" s="13">
-        <f>N15^2</f>
+        <f t="shared" si="0"/>
         <v>6507.1111111111122</v>
       </c>
     </row>
-    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="N16" s="5">
         <v>83.533333333333331</v>
       </c>
       <c r="P16" s="13">
-        <f>N16^2</f>
+        <f t="shared" si="0"/>
         <v>6977.8177777777773</v>
       </c>
     </row>
@@ -4810,7 +5277,7 @@
         <v>84.399999999999991</v>
       </c>
       <c r="P17" s="13">
-        <f>N17^2</f>
+        <f t="shared" si="0"/>
         <v>7123.3599999999988</v>
       </c>
     </row>
@@ -4819,7 +5286,7 @@
         <v>84.600000000000009</v>
       </c>
       <c r="P18" s="13">
-        <f>N18^2</f>
+        <f t="shared" si="0"/>
         <v>7157.1600000000017</v>
       </c>
     </row>
@@ -4828,7 +5295,7 @@
         <v>84.600000000000009</v>
       </c>
       <c r="P19" s="13">
-        <f>N19^2</f>
+        <f t="shared" si="0"/>
         <v>7157.1600000000017</v>
       </c>
     </row>
@@ -4837,7 +5304,7 @@
         <v>85.666666666666671</v>
       </c>
       <c r="P20" s="13">
-        <f>N20^2</f>
+        <f t="shared" si="0"/>
         <v>7338.7777777777783</v>
       </c>
     </row>
@@ -4846,7 +5313,7 @@
         <v>85.733333333333334</v>
       </c>
       <c r="P21" s="13">
-        <f>N21^2</f>
+        <f t="shared" si="0"/>
         <v>7350.2044444444446</v>
       </c>
     </row>
@@ -4855,7 +5322,7 @@
         <v>86</v>
       </c>
       <c r="P22" s="13">
-        <f>N22^2</f>
+        <f t="shared" si="0"/>
         <v>7396</v>
       </c>
     </row>
@@ -4864,7 +5331,7 @@
         <v>86.133333333333326</v>
       </c>
       <c r="P23" s="13">
-        <f>N23^2</f>
+        <f t="shared" si="0"/>
         <v>7418.9511111111096</v>
       </c>
     </row>
@@ -4873,7 +5340,7 @@
         <v>86.333333333333329</v>
       </c>
       <c r="P24" s="13">
-        <f>N24^2</f>
+        <f t="shared" si="0"/>
         <v>7453.4444444444434</v>
       </c>
     </row>
@@ -4882,7 +5349,7 @@
         <v>86.333333333333329</v>
       </c>
       <c r="P25" s="13">
-        <f>N25^2</f>
+        <f t="shared" si="0"/>
         <v>7453.4444444444434</v>
       </c>
     </row>
@@ -4891,7 +5358,7 @@
         <v>86.666666666666671</v>
       </c>
       <c r="P26" s="13">
-        <f>N26^2</f>
+        <f t="shared" si="0"/>
         <v>7511.1111111111122</v>
       </c>
     </row>
@@ -4900,7 +5367,7 @@
         <v>87</v>
       </c>
       <c r="P27" s="13">
-        <f>N27^2</f>
+        <f t="shared" si="0"/>
         <v>7569</v>
       </c>
     </row>
@@ -4909,7 +5376,7 @@
         <v>88.666666666666671</v>
       </c>
       <c r="P28" s="13">
-        <f>N28^2</f>
+        <f t="shared" si="0"/>
         <v>7861.7777777777783</v>
       </c>
     </row>
@@ -4918,7 +5385,7 @@
         <v>89.266666666666666</v>
       </c>
       <c r="P29" s="13">
-        <f>N29^2</f>
+        <f t="shared" si="0"/>
         <v>7968.5377777777776</v>
       </c>
     </row>
@@ -4927,7 +5394,7 @@
         <v>89.466666666666654</v>
       </c>
       <c r="P30" s="13">
-        <f>N30^2</f>
+        <f t="shared" si="0"/>
         <v>8004.2844444444427</v>
       </c>
     </row>
@@ -4936,7 +5403,7 @@
         <v>89.8</v>
       </c>
       <c r="P31" s="13">
-        <f>N31^2</f>
+        <f t="shared" si="0"/>
         <v>8064.0399999999991</v>
       </c>
     </row>
@@ -4945,7 +5412,7 @@
         <v>89.933333333333337</v>
       </c>
       <c r="P32" s="13">
-        <f>N32^2</f>
+        <f t="shared" si="0"/>
         <v>8088.0044444444447</v>
       </c>
     </row>
@@ -4954,7 +5421,7 @@
         <v>90.666666666666671</v>
       </c>
       <c r="P33" s="13">
-        <f>N33^2</f>
+        <f t="shared" si="0"/>
         <v>8220.4444444444453</v>
       </c>
     </row>
@@ -4963,7 +5430,7 @@
         <v>90.8</v>
       </c>
       <c r="P34" s="13">
-        <f>N34^2</f>
+        <f t="shared" si="0"/>
         <v>8244.64</v>
       </c>
     </row>
@@ -4972,7 +5439,7 @@
         <v>90.866666666666674</v>
       </c>
       <c r="P35" s="13">
-        <f>N35^2</f>
+        <f t="shared" si="0"/>
         <v>8256.7511111111126</v>
       </c>
     </row>
@@ -4981,7 +5448,7 @@
         <v>91.066666666666663</v>
       </c>
       <c r="P36" s="13">
-        <f>N36^2</f>
+        <f t="shared" ref="P36:P53" si="3">N36^2</f>
         <v>8293.137777777778</v>
       </c>
     </row>
@@ -4990,7 +5457,7 @@
         <v>91.533333333333346</v>
       </c>
       <c r="P37" s="13">
-        <f>N37^2</f>
+        <f t="shared" si="3"/>
         <v>8378.3511111111129</v>
       </c>
     </row>
@@ -4999,7 +5466,7 @@
         <v>91.533333333333346</v>
       </c>
       <c r="P38" s="13">
-        <f>N38^2</f>
+        <f t="shared" si="3"/>
         <v>8378.3511111111129</v>
       </c>
     </row>
@@ -5008,7 +5475,7 @@
         <v>92</v>
       </c>
       <c r="P39" s="13">
-        <f>N39^2</f>
+        <f t="shared" si="3"/>
         <v>8464</v>
       </c>
     </row>
@@ -5017,7 +5484,7 @@
         <v>92.333333333333329</v>
       </c>
       <c r="P40" s="13">
-        <f>N40^2</f>
+        <f t="shared" si="3"/>
         <v>8525.4444444444434</v>
       </c>
     </row>
@@ -5026,7 +5493,7 @@
         <v>92.733333333333334</v>
       </c>
       <c r="P41" s="13">
-        <f>N41^2</f>
+        <f t="shared" si="3"/>
         <v>8599.4711111111119</v>
       </c>
     </row>
@@ -5035,7 +5502,7 @@
         <v>92.933333333333337</v>
       </c>
       <c r="P42" s="13">
-        <f>N42^2</f>
+        <f t="shared" si="3"/>
         <v>8636.6044444444451</v>
       </c>
     </row>
@@ -5044,7 +5511,7 @@
         <v>93.2</v>
       </c>
       <c r="P43" s="13">
-        <f>N43^2</f>
+        <f t="shared" si="3"/>
         <v>8686.24</v>
       </c>
     </row>
@@ -5053,7 +5520,7 @@
         <v>94</v>
       </c>
       <c r="P44" s="13">
-        <f>N44^2</f>
+        <f t="shared" si="3"/>
         <v>8836</v>
       </c>
     </row>
@@ -5062,7 +5529,7 @@
         <v>94.066666666666663</v>
       </c>
       <c r="P45" s="13">
-        <f>N45^2</f>
+        <f t="shared" si="3"/>
         <v>8848.5377777777776</v>
       </c>
     </row>
@@ -5071,7 +5538,7 @@
         <v>94.133333333333326</v>
       </c>
       <c r="P46" s="13">
-        <f>N46^2</f>
+        <f t="shared" si="3"/>
         <v>8861.0844444444429</v>
       </c>
     </row>
@@ -5080,7 +5547,7 @@
         <v>94.600000000000009</v>
       </c>
       <c r="P47" s="13">
-        <f>N47^2</f>
+        <f t="shared" si="3"/>
         <v>8949.1600000000017</v>
       </c>
     </row>
@@ -5089,7 +5556,7 @@
         <v>94.866666666666674</v>
       </c>
       <c r="P48" s="13">
-        <f>N48^2</f>
+        <f t="shared" si="3"/>
         <v>8999.684444444445</v>
       </c>
     </row>
@@ -5098,7 +5565,7 @@
         <v>95.066666666666663</v>
       </c>
       <c r="P49" s="13">
-        <f>N49^2</f>
+        <f t="shared" si="3"/>
         <v>9037.6711111111108</v>
       </c>
     </row>
@@ -5107,7 +5574,7 @@
         <v>95.666666666666671</v>
       </c>
       <c r="P50" s="13">
-        <f>N50^2</f>
+        <f t="shared" si="3"/>
         <v>9152.1111111111113</v>
       </c>
     </row>
@@ -5116,7 +5583,7 @@
         <v>95.666666666666671</v>
       </c>
       <c r="P51" s="13">
-        <f>N51^2</f>
+        <f t="shared" si="3"/>
         <v>9152.1111111111113</v>
       </c>
     </row>
@@ -5125,7 +5592,7 @@
         <v>96.466666666666654</v>
       </c>
       <c r="P52" s="13">
-        <f>N52^2</f>
+        <f t="shared" si="3"/>
         <v>9305.8177777777746</v>
       </c>
     </row>
@@ -5134,7 +5601,7 @@
         <v>97.066666666666663</v>
       </c>
       <c r="P53" s="13">
-        <f>N53^2</f>
+        <f t="shared" si="3"/>
         <v>9421.9377777777772</v>
       </c>
     </row>
@@ -5147,10 +5614,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="B4:I15"/>
+  <dimension ref="B4:I17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5354,7 +5821,15 @@
       </c>
     </row>
     <row r="15" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D15" s="2" t="s">
+        <v>100</v>
+      </c>
       <c r="H15" s="18"/>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D17" s="2" t="s">
+        <v>101</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5366,8 +5841,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="B1:O64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5385,16 +5860,16 @@
       <c r="G1" s="23"/>
       <c r="H1" s="23"/>
       <c r="L1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="M1">
         <f>2/4*(50+1)</f>
         <v>25.5</v>
       </c>
       <c r="N1" t="s">
-        <v>97</v>
-      </c>
-      <c r="O1" s="45">
+        <v>95</v>
+      </c>
+      <c r="O1" s="42">
         <f>89</f>
         <v>89</v>
       </c>
@@ -5432,16 +5907,16 @@
         <v>51</v>
       </c>
       <c r="L3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="M3">
         <f>1/4*(50+1)</f>
         <v>12.75</v>
       </c>
       <c r="N3" t="s">
-        <v>94</v>
-      </c>
-      <c r="O3" s="45">
+        <v>92</v>
+      </c>
+      <c r="O3" s="42">
         <v>84</v>
       </c>
     </row>
@@ -5474,16 +5949,16 @@
         <v>52</v>
       </c>
       <c r="L4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="M4">
         <f>3/4*(50+1)</f>
         <v>38.25</v>
       </c>
       <c r="N4" t="s">
-        <v>93</v>
-      </c>
-      <c r="O4" s="45">
+        <v>91</v>
+      </c>
+      <c r="O4" s="42">
         <v>93</v>
       </c>
     </row>
@@ -5536,7 +6011,7 @@
       </c>
       <c r="J6" s="29"/>
       <c r="K6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
@@ -5570,10 +6045,10 @@
         <v>82.816666666666663</v>
       </c>
       <c r="L7" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="M7" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="O7">
         <f>(K9-K7)/2</f>
@@ -5606,10 +6081,10 @@
         <v>88.966666666666669</v>
       </c>
       <c r="L8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="M8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.25">
@@ -5643,10 +6118,10 @@
         <v>92.783333333333331</v>
       </c>
       <c r="L9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="M9" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.25">
@@ -5745,11 +6220,11 @@
       </c>
     </row>
     <row r="27" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C27" s="44">
+      <c r="C27" s="41">
         <v>83.533333333333331</v>
       </c>
       <c r="D27" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="28" spans="3:4" x14ac:dyDescent="0.25">
@@ -5808,11 +6283,11 @@
       </c>
     </row>
     <row r="39" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C39" s="46">
+      <c r="C39" s="43">
         <v>88.666666666666671</v>
       </c>
       <c r="D39" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="40" spans="3:4" x14ac:dyDescent="0.25">
@@ -5876,11 +6351,11 @@
       </c>
     </row>
     <row r="52" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C52" s="44">
+      <c r="C52" s="41">
         <v>92.733333333333334</v>
       </c>
       <c r="D52" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="53" spans="3:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Penambahan bagian kuartil, menambah kesimpulan
</commit_message>
<xml_diff>
--- a/Data Penyebaran Data Frekuensi Tugas Kelompok.xlsx
+++ b/Data Penyebaran Data Frekuensi Tugas Kelompok.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hamdi\Documents\statistikafiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA539A3F-742C-4B24-9F84-9A65E962DB1F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2F26C54-DCA4-4BD6-83C4-79E35302777F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="102">
   <si>
     <t>No. Urut</t>
   </si>
@@ -244,12 +244,6 @@
     <t>Kelas Ke-7 (93-98)</t>
   </si>
   <si>
-    <t xml:space="preserve">Jumlah Q1 </t>
-  </si>
-  <si>
-    <t>Jumlah Q3</t>
-  </si>
-  <si>
     <t>Jangkauan Persentil</t>
   </si>
   <si>
@@ -277,9 +271,6 @@
     <t>Jumlah P90</t>
   </si>
   <si>
-    <t>Jangkauan Kuartil</t>
-  </si>
-  <si>
     <t>Kuartil adalah bilangan yang digunakan untuk membagi sekumpulan data menjadi 4 bagian yang jumlahnya sama banyak</t>
   </si>
   <si>
@@ -370,9 +361,6 @@
     <t>Q2</t>
   </si>
   <si>
-    <t>Nilai ke 25</t>
-  </si>
-  <si>
     <t>Rumus Excel</t>
   </si>
   <si>
@@ -392,6 +380,15 @@
   </si>
   <si>
     <t>Varian merupakan ukuran variabilitas data, yang berarti semakin besar nilai varian berarti semakin tinggi fluktuasi data antara satu data dengan data yang lain</t>
+  </si>
+  <si>
+    <t>Nilai ke 26</t>
+  </si>
+  <si>
+    <t>Jangkauan / simpangan Kuartil</t>
+  </si>
+  <si>
+    <t>Simpangan kuartil adalah setengah dari nilai selisih data Kuartil atas dan kuartil bawah</t>
   </si>
 </sst>
 </file>
@@ -730,6 +727,9 @@
     <xf numFmtId="1" fontId="8" fillId="5" borderId="4" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -739,9 +739,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Comma [0] 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -1379,8 +1376,8 @@
       <xdr:rowOff>33337</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="448007" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="TextBox 4">
@@ -1422,6 +1419,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -1479,7 +1477,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="TextBox 4">
@@ -1543,8 +1541,8 @@
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="495300" cy="219163"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="7" name="TextBox 6">
@@ -1621,7 +1619,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="7" name="TextBox 6">
@@ -1687,8 +1685,8 @@
       <xdr:rowOff>185737</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="156133" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="8" name="TextBox 7">
@@ -1730,6 +1728,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -1750,7 +1749,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="8" name="TextBox 7">
@@ -2940,7 +2939,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
@@ -2948,7 +2947,7 @@
       </c>
     </row>
     <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="45"/>
+      <c r="A2" s="48"/>
       <c r="B2" s="8" t="s">
         <v>2</v>
       </c>
@@ -3444,7 +3443,7 @@
         <v>91.066666666666663</v>
       </c>
       <c r="H36" s="35" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I36" s="35"/>
     </row>
@@ -3466,7 +3465,7 @@
         <v>91.533333333333346</v>
       </c>
       <c r="H38" s="33" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="I38" s="33">
         <v>85.705333333333328</v>
@@ -3480,7 +3479,7 @@
         <v>92</v>
       </c>
       <c r="H39" s="33" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="I39" s="33">
         <v>1.4179120928138926</v>
@@ -3494,7 +3493,7 @@
         <v>92.333333333333329</v>
       </c>
       <c r="H40" s="33" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="I40" s="33">
         <v>88.966666666666669</v>
@@ -3508,7 +3507,7 @@
         <v>92.733333333333334</v>
       </c>
       <c r="H41" s="33" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="I41" s="33">
         <v>84.600000000000009</v>
@@ -3522,7 +3521,7 @@
         <v>92.933333333333337</v>
       </c>
       <c r="H42" s="33" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="I42" s="33">
         <v>10.026152559551129</v>
@@ -3536,7 +3535,7 @@
         <v>93.2</v>
       </c>
       <c r="H43" s="33" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="I43" s="33">
         <v>100.52373514739364</v>
@@ -3550,7 +3549,7 @@
         <v>94</v>
       </c>
       <c r="H44" s="33" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="I44" s="33">
         <v>1.4547799557831986</v>
@@ -3564,7 +3563,7 @@
         <v>94.066666666666663</v>
       </c>
       <c r="H45" s="33" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I45" s="33">
         <v>-1.44069540750446</v>
@@ -3578,7 +3577,7 @@
         <v>94.133333333333326</v>
       </c>
       <c r="H46" s="33" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="I46" s="33">
         <v>40.066666666666663</v>
@@ -3592,7 +3591,7 @@
         <v>94.600000000000009</v>
       </c>
       <c r="H47" s="33" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="I47" s="33">
         <v>57</v>
@@ -3606,7 +3605,7 @@
         <v>94.866666666666674</v>
       </c>
       <c r="H48" s="33" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="I48" s="33">
         <v>97.066666666666663</v>
@@ -3620,7 +3619,7 @@
         <v>95.066666666666663</v>
       </c>
       <c r="H49" s="33" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="I49" s="33">
         <v>4285.2666666666664</v>
@@ -3634,7 +3633,7 @@
         <v>95.666666666666671</v>
       </c>
       <c r="H50" s="34" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I50" s="34">
         <v>50</v>
@@ -3684,7 +3683,7 @@
   <dimension ref="B1:S17"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+      <selection activeCell="B10" sqref="B10:K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4199,7 +4198,7 @@
     <row r="17" spans="14:15" x14ac:dyDescent="0.25">
       <c r="N17" s="36"/>
       <c r="O17" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -4230,7 +4229,7 @@
         <v>45</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="2:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -4269,7 +4268,7 @@
       <c r="L5" s="6">
         <v>57</v>
       </c>
-      <c r="M5" s="47">
+      <c r="M5" s="44">
         <f>ABS(L5-$M$3)</f>
         <v>28.705333333333328</v>
       </c>
@@ -4300,7 +4299,7 @@
       <c r="L6" s="5">
         <v>60</v>
       </c>
-      <c r="M6" s="47">
+      <c r="M6" s="44">
         <f t="shared" ref="M6:M54" si="0">ABS(L6-$M$3)</f>
         <v>25.705333333333328</v>
       </c>
@@ -4331,7 +4330,7 @@
       <c r="L7" s="5">
         <v>62</v>
       </c>
-      <c r="M7" s="47">
+      <c r="M7" s="44">
         <f t="shared" si="0"/>
         <v>23.705333333333328</v>
       </c>
@@ -4362,7 +4361,7 @@
       <c r="L8" s="5">
         <v>63.066666666666663</v>
       </c>
-      <c r="M8" s="47">
+      <c r="M8" s="44">
         <f t="shared" si="0"/>
         <v>22.638666666666666</v>
       </c>
@@ -4393,7 +4392,7 @@
       <c r="L9" s="6">
         <v>66</v>
       </c>
-      <c r="M9" s="47">
+      <c r="M9" s="44">
         <f t="shared" si="0"/>
         <v>19.705333333333328</v>
       </c>
@@ -4424,7 +4423,7 @@
       <c r="L10" s="6">
         <v>70</v>
       </c>
-      <c r="M10" s="47">
+      <c r="M10" s="44">
         <f t="shared" si="0"/>
         <v>15.705333333333328</v>
       </c>
@@ -4455,7 +4454,7 @@
       <c r="L11" s="6">
         <v>74</v>
       </c>
-      <c r="M11" s="47">
+      <c r="M11" s="44">
         <f t="shared" si="0"/>
         <v>11.705333333333328</v>
       </c>
@@ -4486,7 +4485,7 @@
       <c r="L12" s="6">
         <v>78</v>
       </c>
-      <c r="M12" s="47">
+      <c r="M12" s="44">
         <f t="shared" si="0"/>
         <v>7.7053333333333285</v>
       </c>
@@ -4512,7 +4511,7 @@
       <c r="L13" s="5">
         <v>79.466666666666669</v>
       </c>
-      <c r="M13" s="47">
+      <c r="M13" s="44">
         <f t="shared" si="0"/>
         <v>6.2386666666666599</v>
       </c>
@@ -4521,7 +4520,7 @@
       <c r="L14" s="6">
         <v>79.666666666666671</v>
       </c>
-      <c r="M14" s="47">
+      <c r="M14" s="44">
         <f t="shared" si="0"/>
         <v>6.0386666666666571</v>
       </c>
@@ -4530,7 +4529,7 @@
       <c r="L15" s="6">
         <v>80</v>
       </c>
-      <c r="M15" s="47">
+      <c r="M15" s="44">
         <f t="shared" si="0"/>
         <v>5.7053333333333285</v>
       </c>
@@ -4543,16 +4542,16 @@
       <c r="L16" s="6">
         <v>80.666666666666671</v>
       </c>
-      <c r="M16" s="47">
+      <c r="M16" s="44">
         <f t="shared" si="0"/>
         <v>5.0386666666666571</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="46" t="s">
+      <c r="A17" s="49" t="s">
         <v>46</v>
       </c>
-      <c r="B17" s="46"/>
+      <c r="B17" s="49"/>
       <c r="C17" s="17" t="s">
         <v>45</v>
       </c>
@@ -4563,31 +4562,31 @@
       <c r="L17" s="5">
         <v>83.533333333333331</v>
       </c>
-      <c r="M17" s="47">
+      <c r="M17" s="44">
         <f t="shared" si="0"/>
         <v>2.171999999999997</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E18" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="L18" s="5">
         <v>84.399999999999991</v>
       </c>
-      <c r="M18" s="47">
+      <c r="M18" s="44">
         <f t="shared" si="0"/>
         <v>1.305333333333337</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="L19" s="5">
         <v>84.600000000000009</v>
       </c>
-      <c r="M19" s="47">
+      <c r="M19" s="44">
         <f t="shared" si="0"/>
         <v>1.10533333333332</v>
       </c>
@@ -4596,7 +4595,7 @@
       <c r="L20" s="5">
         <v>84.600000000000009</v>
       </c>
-      <c r="M20" s="47">
+      <c r="M20" s="44">
         <f t="shared" si="0"/>
         <v>1.10533333333332</v>
       </c>
@@ -4605,7 +4604,7 @@
       <c r="L21" s="6">
         <v>85.666666666666671</v>
       </c>
-      <c r="M21" s="47">
+      <c r="M21" s="44">
         <f t="shared" si="0"/>
         <v>3.8666666666657079E-2</v>
       </c>
@@ -4614,7 +4613,7 @@
       <c r="L22" s="5">
         <v>85.733333333333334</v>
       </c>
-      <c r="M22" s="47">
+      <c r="M22" s="44">
         <f t="shared" si="0"/>
         <v>2.8000000000005798E-2</v>
       </c>
@@ -4623,7 +4622,7 @@
       <c r="L23" s="5">
         <v>86</v>
       </c>
-      <c r="M23" s="47">
+      <c r="M23" s="44">
         <f t="shared" si="0"/>
         <v>0.29466666666667152</v>
       </c>
@@ -4632,7 +4631,7 @@
       <c r="L24" s="5">
         <v>86.133333333333326</v>
       </c>
-      <c r="M24" s="47">
+      <c r="M24" s="44">
         <f t="shared" si="0"/>
         <v>0.42799999999999727</v>
       </c>
@@ -4641,7 +4640,7 @@
       <c r="L25" s="5">
         <v>86.333333333333329</v>
       </c>
-      <c r="M25" s="47">
+      <c r="M25" s="44">
         <f t="shared" si="0"/>
         <v>0.62800000000000011</v>
       </c>
@@ -4650,7 +4649,7 @@
       <c r="L26" s="6">
         <v>86.333333333333329</v>
       </c>
-      <c r="M26" s="47">
+      <c r="M26" s="44">
         <f t="shared" si="0"/>
         <v>0.62800000000000011</v>
       </c>
@@ -4659,7 +4658,7 @@
       <c r="L27" s="5">
         <v>86.666666666666671</v>
       </c>
-      <c r="M27" s="47">
+      <c r="M27" s="44">
         <f t="shared" si="0"/>
         <v>0.96133333333334292</v>
       </c>
@@ -4668,7 +4667,7 @@
       <c r="L28" s="6">
         <v>87</v>
       </c>
-      <c r="M28" s="47">
+      <c r="M28" s="44">
         <f t="shared" si="0"/>
         <v>1.2946666666666715</v>
       </c>
@@ -4677,7 +4676,7 @@
       <c r="L29" s="6">
         <v>88.666666666666671</v>
       </c>
-      <c r="M29" s="47">
+      <c r="M29" s="44">
         <f t="shared" si="0"/>
         <v>2.9613333333333429</v>
       </c>
@@ -4686,7 +4685,7 @@
       <c r="L30" s="5">
         <v>89.266666666666666</v>
       </c>
-      <c r="M30" s="47">
+      <c r="M30" s="44">
         <f t="shared" si="0"/>
         <v>3.5613333333333372</v>
       </c>
@@ -4695,7 +4694,7 @@
       <c r="L31" s="5">
         <v>89.466666666666654</v>
       </c>
-      <c r="M31" s="47">
+      <c r="M31" s="44">
         <f t="shared" si="0"/>
         <v>3.7613333333333259</v>
       </c>
@@ -4704,7 +4703,7 @@
       <c r="L32" s="5">
         <v>89.8</v>
       </c>
-      <c r="M32" s="47">
+      <c r="M32" s="44">
         <f t="shared" si="0"/>
         <v>4.0946666666666687</v>
       </c>
@@ -4713,7 +4712,7 @@
       <c r="L33" s="5">
         <v>89.933333333333337</v>
       </c>
-      <c r="M33" s="47">
+      <c r="M33" s="44">
         <f t="shared" si="0"/>
         <v>4.2280000000000086</v>
       </c>
@@ -4722,7 +4721,7 @@
       <c r="L34" s="5">
         <v>90.666666666666671</v>
       </c>
-      <c r="M34" s="47">
+      <c r="M34" s="44">
         <f t="shared" si="0"/>
         <v>4.9613333333333429</v>
       </c>
@@ -4731,7 +4730,7 @@
       <c r="L35" s="5">
         <v>90.8</v>
       </c>
-      <c r="M35" s="47">
+      <c r="M35" s="44">
         <f t="shared" si="0"/>
         <v>5.0946666666666687</v>
       </c>
@@ -4740,7 +4739,7 @@
       <c r="L36" s="5">
         <v>90.866666666666674</v>
       </c>
-      <c r="M36" s="47">
+      <c r="M36" s="44">
         <f t="shared" si="0"/>
         <v>5.1613333333333458</v>
       </c>
@@ -4749,7 +4748,7 @@
       <c r="L37" s="5">
         <v>91.066666666666663</v>
       </c>
-      <c r="M37" s="47">
+      <c r="M37" s="44">
         <f t="shared" si="0"/>
         <v>5.3613333333333344</v>
       </c>
@@ -4758,7 +4757,7 @@
       <c r="L38" s="5">
         <v>91.533333333333346</v>
       </c>
-      <c r="M38" s="47">
+      <c r="M38" s="44">
         <f t="shared" si="0"/>
         <v>5.8280000000000172</v>
       </c>
@@ -4767,7 +4766,7 @@
       <c r="L39" s="5">
         <v>91.533333333333346</v>
       </c>
-      <c r="M39" s="47">
+      <c r="M39" s="44">
         <f t="shared" si="0"/>
         <v>5.8280000000000172</v>
       </c>
@@ -4776,7 +4775,7 @@
       <c r="L40" s="5">
         <v>92</v>
       </c>
-      <c r="M40" s="47">
+      <c r="M40" s="44">
         <f t="shared" si="0"/>
         <v>6.2946666666666715</v>
       </c>
@@ -4785,7 +4784,7 @@
       <c r="L41" s="5">
         <v>92.333333333333329</v>
       </c>
-      <c r="M41" s="47">
+      <c r="M41" s="44">
         <f t="shared" si="0"/>
         <v>6.6280000000000001</v>
       </c>
@@ -4794,7 +4793,7 @@
       <c r="L42" s="5">
         <v>92.733333333333334</v>
       </c>
-      <c r="M42" s="47">
+      <c r="M42" s="44">
         <f t="shared" si="0"/>
         <v>7.0280000000000058</v>
       </c>
@@ -4803,7 +4802,7 @@
       <c r="L43" s="5">
         <v>92.933333333333337</v>
       </c>
-      <c r="M43" s="47">
+      <c r="M43" s="44">
         <f t="shared" si="0"/>
         <v>7.2280000000000086</v>
       </c>
@@ -4812,7 +4811,7 @@
       <c r="L44" s="5">
         <v>93.2</v>
       </c>
-      <c r="M44" s="47">
+      <c r="M44" s="44">
         <f t="shared" si="0"/>
         <v>7.4946666666666744</v>
       </c>
@@ -4821,7 +4820,7 @@
       <c r="L45" s="5">
         <v>94</v>
       </c>
-      <c r="M45" s="47">
+      <c r="M45" s="44">
         <f t="shared" si="0"/>
         <v>8.2946666666666715</v>
       </c>
@@ -4830,7 +4829,7 @@
       <c r="L46" s="5">
         <v>94.066666666666663</v>
       </c>
-      <c r="M46" s="47">
+      <c r="M46" s="44">
         <f t="shared" si="0"/>
         <v>8.3613333333333344</v>
       </c>
@@ -4839,7 +4838,7 @@
       <c r="L47" s="5">
         <v>94.133333333333326</v>
       </c>
-      <c r="M47" s="47">
+      <c r="M47" s="44">
         <f t="shared" si="0"/>
         <v>8.4279999999999973</v>
       </c>
@@ -4848,7 +4847,7 @@
       <c r="L48" s="5">
         <v>94.600000000000009</v>
       </c>
-      <c r="M48" s="47">
+      <c r="M48" s="44">
         <f t="shared" si="0"/>
         <v>8.89466666666668</v>
       </c>
@@ -4857,7 +4856,7 @@
       <c r="L49" s="5">
         <v>94.866666666666674</v>
       </c>
-      <c r="M49" s="47">
+      <c r="M49" s="44">
         <f t="shared" si="0"/>
         <v>9.1613333333333458</v>
       </c>
@@ -4866,7 +4865,7 @@
       <c r="L50" s="5">
         <v>95.066666666666663</v>
       </c>
-      <c r="M50" s="47">
+      <c r="M50" s="44">
         <f t="shared" si="0"/>
         <v>9.3613333333333344</v>
       </c>
@@ -4875,7 +4874,7 @@
       <c r="L51" s="6">
         <v>95.666666666666671</v>
       </c>
-      <c r="M51" s="47">
+      <c r="M51" s="44">
         <f t="shared" si="0"/>
         <v>9.9613333333333429</v>
       </c>
@@ -4884,7 +4883,7 @@
       <c r="L52" s="6">
         <v>95.666666666666671</v>
       </c>
-      <c r="M52" s="47">
+      <c r="M52" s="44">
         <f t="shared" si="0"/>
         <v>9.9613333333333429</v>
       </c>
@@ -4893,7 +4892,7 @@
       <c r="L53" s="5">
         <v>96.466666666666654</v>
       </c>
-      <c r="M53" s="47">
+      <c r="M53" s="44">
         <f t="shared" si="0"/>
         <v>10.761333333333326</v>
       </c>
@@ -4902,17 +4901,17 @@
       <c r="L54" s="5">
         <v>97.066666666666663</v>
       </c>
-      <c r="M54" s="47">
+      <c r="M54" s="44">
         <f t="shared" si="0"/>
         <v>11.361333333333334</v>
       </c>
     </row>
     <row r="55" spans="12:13" x14ac:dyDescent="0.25">
-      <c r="L55" s="48">
+      <c r="L55" s="45">
         <f>SUM(L5:L54)</f>
         <v>4285.2666666666664</v>
       </c>
-      <c r="M55" s="49">
+      <c r="M55" s="46">
         <f>SUM(M5:M54)</f>
         <v>368.64800000000008</v>
       </c>
@@ -4931,8 +4930,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A3:R53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="N44" sqref="N44:N53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4946,13 +4945,13 @@
   <sheetData>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="O3" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
@@ -5132,7 +5131,7 @@
         <v>83.5</v>
       </c>
       <c r="H9" s="18" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="I9" s="2">
         <f>((50*Variansi!Q4)-Variansi!R4)/(50*49)</f>
@@ -5193,7 +5192,7 @@
         <v>95.5</v>
       </c>
       <c r="H11" s="18" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="I11" s="2">
         <f>SQRT(I9)</f>
@@ -5253,7 +5252,7 @@
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="N15" s="6">
         <v>80.666666666666671</v>
@@ -5616,7 +5615,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B4:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
@@ -5822,13 +5821,13 @@
     </row>
     <row r="15" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="D15" s="2" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="H15" s="18"/>
     </row>
     <row r="17" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D17" s="2" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -5841,8 +5840,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="B1:O64"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5850,7 +5849,7 @@
     <col min="2" max="2" width="9.85546875" customWidth="1"/>
     <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="31.140625" customWidth="1"/>
     <col min="10" max="10" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -5860,14 +5859,14 @@
       <c r="G1" s="23"/>
       <c r="H1" s="23"/>
       <c r="L1" t="s">
-        <v>93</v>
-      </c>
-      <c r="M1">
-        <f>2/4*(50+1)</f>
+        <v>90</v>
+      </c>
+      <c r="M1" s="13">
+        <f>((50/2) + (50/2 + 1))/2</f>
         <v>25.5</v>
       </c>
       <c r="N1" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="O1" s="42">
         <f>89</f>
@@ -5897,7 +5896,7 @@
       </c>
       <c r="G3" s="23"/>
       <c r="H3" s="25" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I3" s="26">
         <f>1/4 *50</f>
@@ -5907,14 +5906,14 @@
         <v>51</v>
       </c>
       <c r="L3" t="s">
+        <v>86</v>
+      </c>
+      <c r="M3">
+        <f>(50+2)/4</f>
+        <v>13</v>
+      </c>
+      <c r="N3" t="s">
         <v>89</v>
-      </c>
-      <c r="M3">
-        <f>1/4*(50+1)</f>
-        <v>12.75</v>
-      </c>
-      <c r="N3" t="s">
-        <v>92</v>
       </c>
       <c r="O3" s="42">
         <v>84</v>
@@ -5939,7 +5938,7 @@
         <v>6</v>
       </c>
       <c r="H4" s="26" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I4" s="26">
         <f>3/4 *50</f>
@@ -5949,14 +5948,14 @@
         <v>52</v>
       </c>
       <c r="L4" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="M4">
-        <f>3/4*(50+1)</f>
-        <v>38.25</v>
+        <f>(3*50+2)/4</f>
+        <v>38</v>
       </c>
       <c r="N4" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="O4" s="42">
         <v>93</v>
@@ -6002,16 +6001,11 @@
       <c r="F6" s="16">
         <v>6</v>
       </c>
-      <c r="H6" s="26" t="s">
-        <v>53</v>
-      </c>
-      <c r="I6" s="28">
-        <f>D8+(((1/4*C11)-SUM(C4:C7))/C8)*F8</f>
-        <v>81.318181818181813</v>
-      </c>
+      <c r="H6" s="26"/>
+      <c r="I6" s="28"/>
       <c r="J6" s="29"/>
       <c r="K6" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
@@ -6032,23 +6026,18 @@
       <c r="F7" s="16">
         <v>6</v>
       </c>
-      <c r="H7" s="26" t="s">
-        <v>54</v>
-      </c>
-      <c r="I7" s="30">
-        <f>D10+(((3/4*C11)-SUM(C4:C9))/C10)*F10</f>
-        <v>92.730769230769226</v>
-      </c>
+      <c r="H7" s="26"/>
+      <c r="I7" s="30"/>
       <c r="J7" s="26"/>
       <c r="K7">
         <f>_xlfn.QUARTILE.EXC($C$15:$C$64,1)</f>
         <v>82.816666666666663</v>
       </c>
       <c r="L7" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="M7" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="O7">
         <f>(K9-K7)/2</f>
@@ -6081,10 +6070,10 @@
         <v>88.966666666666669</v>
       </c>
       <c r="L8" t="s">
+        <v>91</v>
+      </c>
+      <c r="M8" t="s">
         <v>94</v>
-      </c>
-      <c r="M8" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.25">
@@ -6106,11 +6095,11 @@
         <v>6</v>
       </c>
       <c r="H9" s="26" t="s">
-        <v>64</v>
+        <v>100</v>
       </c>
       <c r="I9" s="28">
-        <f>1/2*(I7-I6)</f>
-        <v>5.7062937062937067</v>
+        <f xml:space="preserve"> (O4 - O3)/2</f>
+        <v>4.5</v>
       </c>
       <c r="J9" s="26"/>
       <c r="K9" s="2">
@@ -6118,10 +6107,10 @@
         <v>92.783333333333331</v>
       </c>
       <c r="L9" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="M9" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.25">
@@ -6156,7 +6145,12 @@
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.25">
       <c r="H12" t="s">
-        <v>65</v>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="H13" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.25">
@@ -6224,7 +6218,7 @@
         <v>83.533333333333331</v>
       </c>
       <c r="D27" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="28" spans="3:4" x14ac:dyDescent="0.25">
@@ -6287,7 +6281,7 @@
         <v>88.666666666666671</v>
       </c>
       <c r="D39" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="40" spans="3:4" x14ac:dyDescent="0.25">
@@ -6355,7 +6349,7 @@
         <v>92.733333333333334</v>
       </c>
       <c r="D52" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="53" spans="3:4" x14ac:dyDescent="0.25">
@@ -6454,14 +6448,14 @@
         <v>50</v>
       </c>
       <c r="H3" s="24" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="I3" s="31">
         <f>10/100*C11</f>
         <v>5</v>
       </c>
       <c r="J3" s="31" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="K3" s="31"/>
     </row>
@@ -6484,14 +6478,14 @@
         <v>6</v>
       </c>
       <c r="H4" s="31" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I4" s="31">
         <f>90/100*C11</f>
         <v>45</v>
       </c>
       <c r="J4" s="31" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="K4" s="31"/>
     </row>
@@ -6537,7 +6531,7 @@
         <v>6</v>
       </c>
       <c r="H6" s="31" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I6" s="32">
         <f>D5+(((10/100*C11)-C4)*F4)/C5</f>
@@ -6565,7 +6559,7 @@
         <v>6</v>
       </c>
       <c r="H7" s="31" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I7" s="32">
         <f>D10+(((90/100*C11)-SUM(C4:C9))*F10)/C10</f>
@@ -6616,7 +6610,7 @@
         <v>6</v>
       </c>
       <c r="H9" s="31" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I9" s="32">
         <f>1/2*(I7-I6)</f>

</xml_diff>

<commit_message>
Penambahan kesimpulan, perbaikan tabel, minus penutup.
</commit_message>
<xml_diff>
--- a/Data Penyebaran Data Frekuensi Tugas Kelompok.xlsx
+++ b/Data Penyebaran Data Frekuensi Tugas Kelompok.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hamdi\Documents\statistikafiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2F26C54-DCA4-4BD6-83C4-79E35302777F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10BACA70-B8CD-4CA9-9CF3-3B7ECF5B695A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1371,13 +1371,13 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>561975</xdr:colOff>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>33337</xdr:rowOff>
+      <xdr:rowOff>4762</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="448007" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="TextBox 4">
@@ -1391,7 +1391,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="8391525" y="604837"/>
+              <a:off x="8029575" y="576262"/>
               <a:ext cx="448007" cy="172227"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -1477,7 +1477,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="TextBox 4">
@@ -1491,7 +1491,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="8391525" y="604837"/>
+              <a:off x="8029575" y="576262"/>
               <a:ext cx="448007" cy="172227"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -1519,6 +1519,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a:r>
                 <a:rPr lang="en-ID" sz="1100" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
@@ -4210,8 +4211,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A2:R55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4219,7 +4220,7 @@
     <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.42578125" customWidth="1"/>
     <col min="7" max="7" width="14.28515625" customWidth="1"/>
-    <col min="13" max="13" width="21.140625" style="40" customWidth="1"/>
+    <col min="13" max="13" width="13.42578125" style="40" customWidth="1"/>
     <col min="16" max="16" width="9.140625" style="40"/>
   </cols>
   <sheetData>
@@ -5840,7 +5841,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="B1:O64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>

</xml_diff>